<commit_message>
Matrix solution, broken search.
</commit_message>
<xml_diff>
--- a/20441/maman16/Drawing.xlsx
+++ b/20441/maman16/Drawing.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="8130"/>
   </bookViews>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>rows</t>
   </si>
@@ -30,7 +29,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -38,13 +37,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,8 +74,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="75">
     <border>
       <left/>
       <right/>
@@ -349,11 +390,730 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -381,8 +1141,274 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,20 +1704,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z20"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AN20"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.625" style="21"/>
-    <col min="17" max="17" width="3.875" customWidth="1"/>
+    <col min="1" max="7" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" style="21"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="21" max="28" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5" style="31" bestFit="1" customWidth="1"/>
+    <col min="30" max="36" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" thickBot="1">
+    <row r="1" spans="1:40" ht="15.75" thickBot="1">
       <c r="A1" s="3">
         <v>16</v>
       </c>
@@ -740,8 +1771,56 @@
       <c r="P1" s="3">
         <v>1</v>
       </c>
+      <c r="U1" s="3">
+        <v>16</v>
+      </c>
+      <c r="V1" s="3">
+        <v>15</v>
+      </c>
+      <c r="W1" s="3">
+        <v>14</v>
+      </c>
+      <c r="X1" s="3">
+        <v>13</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>11</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="35">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="32">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>7</v>
+      </c>
+      <c r="AE1" s="3">
+        <v>6</v>
+      </c>
+      <c r="AF1" s="3">
+        <v>5</v>
+      </c>
+      <c r="AG1" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH1" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI1" s="3">
+        <v>2</v>
+      </c>
+      <c r="AJ1" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:40" ht="15.75" thickBot="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -761,29 +1840,163 @@
       <c r="Q2">
         <v>1</v>
       </c>
+      <c r="U2" s="27">
+        <f t="shared" ref="U2:AA9" si="0">AC2+100</f>
+        <v>-358</v>
+      </c>
+      <c r="V2" s="79">
+        <f t="shared" si="0"/>
+        <v>-360</v>
+      </c>
+      <c r="W2" s="50">
+        <f t="shared" si="0"/>
+        <v>-366</v>
+      </c>
+      <c r="X2" s="55">
+        <f t="shared" si="0"/>
+        <v>-368</v>
+      </c>
+      <c r="Y2" s="50">
+        <f t="shared" si="0"/>
+        <v>-389</v>
+      </c>
+      <c r="Z2" s="79">
+        <f t="shared" si="0"/>
+        <v>-391</v>
+      </c>
+      <c r="AA2" s="50">
+        <f t="shared" si="0"/>
+        <v>-398</v>
+      </c>
+      <c r="AB2" s="64">
+        <f>AJ2+100</f>
+        <v>-400</v>
+      </c>
+      <c r="AC2" s="33">
+        <v>-458</v>
+      </c>
+      <c r="AD2" s="95">
+        <v>-460</v>
+      </c>
+      <c r="AE2" s="33">
+        <v>-466</v>
+      </c>
+      <c r="AF2" s="60">
+        <v>-468</v>
+      </c>
+      <c r="AG2" s="46">
+        <v>-489</v>
+      </c>
+      <c r="AH2" s="74">
+        <v>-491</v>
+      </c>
+      <c r="AI2" s="46">
+        <v>-498</v>
+      </c>
+      <c r="AJ2" s="28">
+        <v>-500</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:26">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:40" ht="15.75" thickBot="1">
+      <c r="A3" s="19"/>
+      <c r="B3" s="123">
+        <v>5</v>
+      </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="123">
+        <v>5</v>
+      </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="123">
+        <v>5</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="122">
+        <v>5</v>
+      </c>
       <c r="I3" s="19"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="123">
+        <v>5</v>
+      </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="123">
+        <v>5</v>
+      </c>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="N3" s="123">
+        <v>5</v>
+      </c>
       <c r="O3" s="1"/>
-      <c r="P3" s="8"/>
+      <c r="P3" s="122">
+        <v>5</v>
+      </c>
       <c r="Q3">
         <v>2</v>
       </c>
+      <c r="U3" s="86">
+        <f t="shared" si="0"/>
+        <v>-357</v>
+      </c>
+      <c r="V3" s="101">
+        <f t="shared" si="0"/>
+        <v>-359</v>
+      </c>
+      <c r="W3" s="88">
+        <f t="shared" si="0"/>
+        <v>-365</v>
+      </c>
+      <c r="X3" s="87">
+        <f t="shared" si="0"/>
+        <v>-367</v>
+      </c>
+      <c r="Y3" s="88">
+        <f t="shared" si="0"/>
+        <v>-388</v>
+      </c>
+      <c r="Z3" s="101">
+        <f t="shared" si="0"/>
+        <v>-390</v>
+      </c>
+      <c r="AA3" s="88">
+        <f t="shared" si="0"/>
+        <v>-397</v>
+      </c>
+      <c r="AB3" s="89">
+        <f t="shared" ref="AB3:AB9" si="1">AJ3+100</f>
+        <v>-399</v>
+      </c>
+      <c r="AC3" s="90">
+        <v>-457</v>
+      </c>
+      <c r="AD3" s="96">
+        <v>-459</v>
+      </c>
+      <c r="AE3" s="90">
+        <v>-465</v>
+      </c>
+      <c r="AF3" s="91">
+        <v>-467</v>
+      </c>
+      <c r="AG3" s="92">
+        <v>-488</v>
+      </c>
+      <c r="AH3" s="93">
+        <v>-490</v>
+      </c>
+      <c r="AI3" s="92">
+        <v>-497</v>
+      </c>
+      <c r="AJ3" s="94">
+        <v>-499</v>
+      </c>
+      <c r="AK3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A4" s="7"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -803,37 +2016,167 @@
       <c r="Q4">
         <v>3</v>
       </c>
+      <c r="U4" s="45">
+        <f t="shared" si="0"/>
+        <v>-354</v>
+      </c>
+      <c r="V4" s="78">
+        <f t="shared" si="0"/>
+        <v>-356</v>
+      </c>
+      <c r="W4" s="51">
+        <f t="shared" si="0"/>
+        <v>-363</v>
+      </c>
+      <c r="X4" s="57">
+        <f t="shared" si="0"/>
+        <v>-364</v>
+      </c>
+      <c r="Y4" s="51">
+        <f t="shared" si="0"/>
+        <v>-385</v>
+      </c>
+      <c r="Z4" s="78">
+        <f t="shared" si="0"/>
+        <v>-387</v>
+      </c>
+      <c r="AA4" s="51">
+        <f t="shared" si="0"/>
+        <v>-393</v>
+      </c>
+      <c r="AB4" s="66">
+        <f t="shared" si="1"/>
+        <v>-395</v>
+      </c>
+      <c r="AC4" s="81">
+        <v>-454</v>
+      </c>
+      <c r="AD4" s="97">
+        <v>-456</v>
+      </c>
+      <c r="AE4" s="81">
+        <v>-463</v>
+      </c>
+      <c r="AF4" s="82">
+        <v>-464</v>
+      </c>
+      <c r="AG4" s="83">
+        <v>-485</v>
+      </c>
+      <c r="AH4" s="84">
+        <v>-487</v>
+      </c>
+      <c r="AI4" s="83">
+        <v>-493</v>
+      </c>
+      <c r="AJ4" s="85">
+        <v>-495</v>
+      </c>
+      <c r="AK4">
+        <v>3</v>
+      </c>
+      <c r="AM4" s="44"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="26">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="C5" s="120">
+        <v>4</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="24">
         <v>3</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="120">
+        <v>4</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="25">
         <v>3</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="K5" s="120">
+        <v>4</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="24">
         <v>3</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="O5" s="120">
+        <v>4</v>
+      </c>
       <c r="P5" s="8"/>
       <c r="Q5">
         <v>4</v>
       </c>
+      <c r="U5" s="118">
+        <f t="shared" si="0"/>
+        <v>-353</v>
+      </c>
+      <c r="V5" s="80">
+        <f t="shared" si="0"/>
+        <v>-355</v>
+      </c>
+      <c r="W5" s="52">
+        <f t="shared" si="0"/>
+        <v>-361</v>
+      </c>
+      <c r="X5" s="56">
+        <f t="shared" si="0"/>
+        <v>-362</v>
+      </c>
+      <c r="Y5" s="117">
+        <f t="shared" si="0"/>
+        <v>-384</v>
+      </c>
+      <c r="Z5" s="80">
+        <f t="shared" si="0"/>
+        <v>-386</v>
+      </c>
+      <c r="AA5" s="52">
+        <f t="shared" si="0"/>
+        <v>-392</v>
+      </c>
+      <c r="AB5" s="65">
+        <f t="shared" si="1"/>
+        <v>-394</v>
+      </c>
+      <c r="AC5" s="116">
+        <v>-453</v>
+      </c>
+      <c r="AD5" s="98">
+        <v>-455</v>
+      </c>
+      <c r="AE5" s="63">
+        <v>-461</v>
+      </c>
+      <c r="AF5" s="61">
+        <v>-462</v>
+      </c>
+      <c r="AG5" s="116">
+        <v>-484</v>
+      </c>
+      <c r="AH5" s="75">
+        <v>-486</v>
+      </c>
+      <c r="AI5" s="53">
+        <v>-492</v>
+      </c>
+      <c r="AJ5" s="54">
+        <v>-494</v>
+      </c>
+      <c r="AK5">
+        <v>4</v>
+      </c>
+      <c r="AL5" s="43"/>
+      <c r="AM5" s="38"/>
+      <c r="AN5" s="39"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A6" s="7"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -853,29 +2196,167 @@
       <c r="Q6">
         <v>5</v>
       </c>
+      <c r="U6" s="45">
+        <f t="shared" si="0"/>
+        <v>-342</v>
+      </c>
+      <c r="V6" s="78">
+        <f t="shared" si="0"/>
+        <v>-344</v>
+      </c>
+      <c r="W6" s="51">
+        <f t="shared" si="0"/>
+        <v>-350</v>
+      </c>
+      <c r="X6" s="57">
+        <f t="shared" si="0"/>
+        <v>-352</v>
+      </c>
+      <c r="Y6" s="51">
+        <f t="shared" si="0"/>
+        <v>-373</v>
+      </c>
+      <c r="Z6" s="78">
+        <f t="shared" si="0"/>
+        <v>-375</v>
+      </c>
+      <c r="AA6" s="51">
+        <f t="shared" si="0"/>
+        <v>-381</v>
+      </c>
+      <c r="AB6" s="66">
+        <f t="shared" si="1"/>
+        <v>-383</v>
+      </c>
+      <c r="AC6" s="47">
+        <v>-442</v>
+      </c>
+      <c r="AD6" s="99">
+        <v>-444</v>
+      </c>
+      <c r="AE6" s="47">
+        <v>-450</v>
+      </c>
+      <c r="AF6" s="62">
+        <v>-452</v>
+      </c>
+      <c r="AG6" s="48">
+        <v>-473</v>
+      </c>
+      <c r="AH6" s="76">
+        <v>-475</v>
+      </c>
+      <c r="AI6" s="48">
+        <v>-481</v>
+      </c>
+      <c r="AJ6" s="49">
+        <v>-483</v>
+      </c>
+      <c r="AK6">
+        <v>5</v>
+      </c>
+      <c r="AM6" s="21"/>
+      <c r="AN6" s="40"/>
     </row>
-    <row r="7" spans="1:26">
-      <c r="A7" s="7"/>
-      <c r="B7" s="1"/>
+    <row r="7" spans="1:40" ht="15.75" thickBot="1">
+      <c r="A7" s="19"/>
+      <c r="B7" s="123">
+        <v>5</v>
+      </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="123">
+        <v>5</v>
+      </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="123">
+        <v>5</v>
+      </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="122">
+        <v>5</v>
+      </c>
       <c r="I7" s="19"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="123">
+        <v>5</v>
+      </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="123">
+        <v>5</v>
+      </c>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="123">
+        <v>5</v>
+      </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="8"/>
+      <c r="P7" s="122">
+        <v>5</v>
+      </c>
       <c r="Q7">
         <v>6</v>
       </c>
+      <c r="U7" s="86">
+        <f t="shared" si="0"/>
+        <v>-341</v>
+      </c>
+      <c r="V7" s="101">
+        <f t="shared" si="0"/>
+        <v>-343</v>
+      </c>
+      <c r="W7" s="88">
+        <f t="shared" si="0"/>
+        <v>-349</v>
+      </c>
+      <c r="X7" s="87">
+        <f t="shared" si="0"/>
+        <v>-351</v>
+      </c>
+      <c r="Y7" s="88">
+        <f t="shared" si="0"/>
+        <v>-372</v>
+      </c>
+      <c r="Z7" s="101">
+        <f t="shared" si="0"/>
+        <v>-374</v>
+      </c>
+      <c r="AA7" s="88">
+        <f t="shared" si="0"/>
+        <v>-380</v>
+      </c>
+      <c r="AB7" s="89">
+        <f t="shared" si="1"/>
+        <v>-382</v>
+      </c>
+      <c r="AC7" s="105">
+        <v>-441</v>
+      </c>
+      <c r="AD7" s="106">
+        <v>-443</v>
+      </c>
+      <c r="AE7" s="105">
+        <v>-449</v>
+      </c>
+      <c r="AF7" s="107">
+        <v>-451</v>
+      </c>
+      <c r="AG7" s="108">
+        <v>-472</v>
+      </c>
+      <c r="AH7" s="109">
+        <v>-474</v>
+      </c>
+      <c r="AI7" s="108">
+        <v>-480</v>
+      </c>
+      <c r="AJ7" s="110">
+        <v>-482</v>
+      </c>
+      <c r="AK7">
+        <v>6</v>
+      </c>
+      <c r="AM7" s="21"/>
+      <c r="AN7" s="40"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A8" s="7"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -895,41 +2376,173 @@
       <c r="Q8">
         <v>7</v>
       </c>
-      <c r="R8" s="27" t="s">
+      <c r="R8" s="30" t="s">
         <v>0</v>
       </c>
+      <c r="U8" s="45">
+        <f t="shared" si="0"/>
+        <v>-338</v>
+      </c>
+      <c r="V8" s="78">
+        <f t="shared" si="0"/>
+        <v>-340</v>
+      </c>
+      <c r="W8" s="51">
+        <f t="shared" si="0"/>
+        <v>-346</v>
+      </c>
+      <c r="X8" s="57">
+        <f t="shared" si="0"/>
+        <v>-348</v>
+      </c>
+      <c r="Y8" s="51">
+        <f t="shared" si="0"/>
+        <v>-370</v>
+      </c>
+      <c r="Z8" s="78">
+        <f t="shared" si="0"/>
+        <v>-372</v>
+      </c>
+      <c r="AA8" s="51">
+        <f t="shared" si="0"/>
+        <v>-377</v>
+      </c>
+      <c r="AB8" s="66">
+        <f t="shared" si="1"/>
+        <v>-379</v>
+      </c>
+      <c r="AC8" s="47">
+        <v>-438</v>
+      </c>
+      <c r="AD8" s="99">
+        <v>-440</v>
+      </c>
+      <c r="AE8" s="47">
+        <v>-446</v>
+      </c>
+      <c r="AF8" s="62">
+        <v>-448</v>
+      </c>
+      <c r="AG8" s="48">
+        <v>-470</v>
+      </c>
+      <c r="AH8" s="76">
+        <v>-472</v>
+      </c>
+      <c r="AI8" s="48">
+        <v>-477</v>
+      </c>
+      <c r="AJ8" s="49">
+        <v>-479</v>
+      </c>
+      <c r="AK8">
+        <v>7</v>
+      </c>
+      <c r="AL8" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="41"/>
+      <c r="AN8" s="42"/>
     </row>
-    <row r="9" spans="1:26" ht="15" thickBot="1">
+    <row r="9" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A9" s="13">
         <v>1</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="C9" s="121">
+        <v>4</v>
+      </c>
       <c r="D9" s="10"/>
       <c r="E9" s="14">
         <v>2</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="G9" s="121">
+        <v>4</v>
+      </c>
       <c r="H9" s="16"/>
       <c r="I9" s="20">
         <v>1</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="K9" s="120">
+        <v>4</v>
+      </c>
       <c r="L9" s="10"/>
       <c r="M9" s="14">
         <v>2</v>
       </c>
       <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+      <c r="O9" s="121">
+        <v>4</v>
+      </c>
       <c r="P9" s="11"/>
       <c r="Q9">
         <v>8</v>
       </c>
-      <c r="R9" s="27"/>
+      <c r="R9" s="30"/>
+      <c r="U9" s="125">
+        <f t="shared" si="0"/>
+        <v>-337</v>
+      </c>
+      <c r="V9" s="102">
+        <f t="shared" si="0"/>
+        <v>-339</v>
+      </c>
+      <c r="W9" s="68">
+        <f t="shared" si="0"/>
+        <v>-345</v>
+      </c>
+      <c r="X9" s="67">
+        <f t="shared" si="0"/>
+        <v>-347</v>
+      </c>
+      <c r="Y9" s="113">
+        <f t="shared" si="0"/>
+        <v>-369</v>
+      </c>
+      <c r="Z9" s="102">
+        <f t="shared" si="0"/>
+        <v>-371</v>
+      </c>
+      <c r="AA9" s="68">
+        <f t="shared" si="0"/>
+        <v>-376</v>
+      </c>
+      <c r="AB9" s="69">
+        <f t="shared" si="1"/>
+        <v>-378</v>
+      </c>
+      <c r="AC9" s="124">
+        <v>-437</v>
+      </c>
+      <c r="AD9" s="100">
+        <v>-439</v>
+      </c>
+      <c r="AE9" s="70">
+        <v>-445</v>
+      </c>
+      <c r="AF9" s="71">
+        <v>-447</v>
+      </c>
+      <c r="AG9" s="112">
+        <v>-469</v>
+      </c>
+      <c r="AH9" s="77">
+        <v>-471</v>
+      </c>
+      <c r="AI9" s="72">
+        <v>-476</v>
+      </c>
+      <c r="AJ9" s="73">
+        <v>-478</v>
+      </c>
+      <c r="AK9">
+        <v>8</v>
+      </c>
+      <c r="AL9" s="30"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:40" ht="15.75" thickBot="1">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -949,31 +2562,183 @@
       <c r="Q10">
         <v>9</v>
       </c>
-      <c r="R10" s="27"/>
+      <c r="R10" s="30"/>
+      <c r="U10" s="45">
+        <f t="shared" ref="U10:AA17" si="2">AC2+150</f>
+        <v>-308</v>
+      </c>
+      <c r="V10" s="78">
+        <f t="shared" si="2"/>
+        <v>-310</v>
+      </c>
+      <c r="W10" s="51">
+        <f t="shared" si="2"/>
+        <v>-316</v>
+      </c>
+      <c r="X10" s="57">
+        <f t="shared" si="2"/>
+        <v>-318</v>
+      </c>
+      <c r="Y10" s="51">
+        <f t="shared" si="2"/>
+        <v>-339</v>
+      </c>
+      <c r="Z10" s="78">
+        <f t="shared" si="2"/>
+        <v>-341</v>
+      </c>
+      <c r="AA10" s="51">
+        <f t="shared" si="2"/>
+        <v>-348</v>
+      </c>
+      <c r="AB10" s="66">
+        <f>AJ2+150</f>
+        <v>-350</v>
+      </c>
+      <c r="AC10" s="36">
+        <f t="shared" ref="AC10:AI17" si="3">AC2+50</f>
+        <v>-408</v>
+      </c>
+      <c r="AD10" s="78">
+        <f t="shared" si="3"/>
+        <v>-410</v>
+      </c>
+      <c r="AE10" s="36">
+        <f t="shared" si="3"/>
+        <v>-416</v>
+      </c>
+      <c r="AF10" s="57">
+        <f t="shared" si="3"/>
+        <v>-418</v>
+      </c>
+      <c r="AG10" s="36">
+        <f t="shared" si="3"/>
+        <v>-439</v>
+      </c>
+      <c r="AH10" s="78">
+        <f t="shared" si="3"/>
+        <v>-441</v>
+      </c>
+      <c r="AI10" s="36">
+        <f t="shared" si="3"/>
+        <v>-448</v>
+      </c>
+      <c r="AJ10" s="37">
+        <f>AJ2+50</f>
+        <v>-450</v>
+      </c>
+      <c r="AK10">
+        <v>9</v>
+      </c>
+      <c r="AL10" s="30"/>
     </row>
-    <row r="11" spans="1:26">
-      <c r="A11" s="7"/>
-      <c r="B11" s="1"/>
+    <row r="11" spans="1:40" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A11" s="19"/>
+      <c r="B11" s="123">
+        <v>5</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="123">
+        <v>5</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="123">
+        <v>5</v>
+      </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="122">
+        <v>5</v>
+      </c>
       <c r="I11" s="19"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="123">
+        <v>5</v>
+      </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="123">
+        <v>5</v>
+      </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="N11" s="123">
+        <v>5</v>
+      </c>
       <c r="O11" s="1"/>
-      <c r="P11" s="8"/>
+      <c r="P11" s="122">
+        <v>5</v>
+      </c>
       <c r="Q11">
         <v>10</v>
       </c>
-      <c r="R11" s="27"/>
+      <c r="R11" s="30"/>
+      <c r="U11" s="86">
+        <f t="shared" si="2"/>
+        <v>-307</v>
+      </c>
+      <c r="V11" s="101">
+        <f t="shared" si="2"/>
+        <v>-309</v>
+      </c>
+      <c r="W11" s="88">
+        <f t="shared" si="2"/>
+        <v>-315</v>
+      </c>
+      <c r="X11" s="87">
+        <f t="shared" si="2"/>
+        <v>-317</v>
+      </c>
+      <c r="Y11" s="88">
+        <f t="shared" si="2"/>
+        <v>-338</v>
+      </c>
+      <c r="Z11" s="101">
+        <f t="shared" si="2"/>
+        <v>-340</v>
+      </c>
+      <c r="AA11" s="88">
+        <f t="shared" si="2"/>
+        <v>-347</v>
+      </c>
+      <c r="AB11" s="89">
+        <f t="shared" ref="AB11:AB17" si="4">AJ3+150</f>
+        <v>-349</v>
+      </c>
+      <c r="AC11" s="103">
+        <f t="shared" si="3"/>
+        <v>-407</v>
+      </c>
+      <c r="AD11" s="101">
+        <f t="shared" si="3"/>
+        <v>-409</v>
+      </c>
+      <c r="AE11" s="103">
+        <f t="shared" si="3"/>
+        <v>-415</v>
+      </c>
+      <c r="AF11" s="87">
+        <f t="shared" si="3"/>
+        <v>-417</v>
+      </c>
+      <c r="AG11" s="103">
+        <f t="shared" si="3"/>
+        <v>-438</v>
+      </c>
+      <c r="AH11" s="101">
+        <f t="shared" si="3"/>
+        <v>-440</v>
+      </c>
+      <c r="AI11" s="103">
+        <f t="shared" si="3"/>
+        <v>-447</v>
+      </c>
+      <c r="AJ11" s="104">
+        <f t="shared" ref="AJ11:AJ17" si="5">AJ3+50</f>
+        <v>-449</v>
+      </c>
+      <c r="AK11">
+        <v>10</v>
+      </c>
+      <c r="AL11" s="30"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A12" s="7"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -993,39 +2758,183 @@
       <c r="Q12">
         <v>11</v>
       </c>
-      <c r="R12" s="27"/>
+      <c r="R12" s="30"/>
+      <c r="U12" s="45">
+        <f t="shared" si="2"/>
+        <v>-304</v>
+      </c>
+      <c r="V12" s="78">
+        <f t="shared" si="2"/>
+        <v>-306</v>
+      </c>
+      <c r="W12" s="51">
+        <f t="shared" si="2"/>
+        <v>-313</v>
+      </c>
+      <c r="X12" s="57">
+        <f t="shared" si="2"/>
+        <v>-314</v>
+      </c>
+      <c r="Y12" s="51">
+        <f t="shared" si="2"/>
+        <v>-335</v>
+      </c>
+      <c r="Z12" s="78">
+        <f t="shared" si="2"/>
+        <v>-337</v>
+      </c>
+      <c r="AA12" s="51">
+        <f t="shared" si="2"/>
+        <v>-343</v>
+      </c>
+      <c r="AB12" s="66">
+        <f t="shared" si="4"/>
+        <v>-345</v>
+      </c>
+      <c r="AC12" s="36">
+        <f t="shared" si="3"/>
+        <v>-404</v>
+      </c>
+      <c r="AD12" s="78">
+        <f t="shared" si="3"/>
+        <v>-406</v>
+      </c>
+      <c r="AE12" s="36">
+        <f t="shared" si="3"/>
+        <v>-413</v>
+      </c>
+      <c r="AF12" s="57">
+        <f t="shared" si="3"/>
+        <v>-414</v>
+      </c>
+      <c r="AG12" s="36">
+        <f t="shared" si="3"/>
+        <v>-435</v>
+      </c>
+      <c r="AH12" s="78">
+        <f t="shared" si="3"/>
+        <v>-437</v>
+      </c>
+      <c r="AI12" s="36">
+        <f t="shared" si="3"/>
+        <v>-443</v>
+      </c>
+      <c r="AJ12" s="37">
+        <f t="shared" si="5"/>
+        <v>-445</v>
+      </c>
+      <c r="AK12">
+        <v>11</v>
+      </c>
+      <c r="AL12" s="30"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:40" ht="15.75" thickBot="1">
       <c r="A13" s="24">
         <v>3</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="120">
+        <v>4</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="24">
         <v>3</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="120">
+        <v>4</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="24">
         <v>3</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="K13" s="120">
+        <v>4</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="24">
         <v>3</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+      <c r="O13" s="120">
+        <v>4</v>
+      </c>
       <c r="P13" s="8"/>
       <c r="Q13">
         <v>12</v>
       </c>
-      <c r="R13" s="27"/>
+      <c r="R13" s="30"/>
+      <c r="U13" s="118">
+        <f t="shared" si="2"/>
+        <v>-303</v>
+      </c>
+      <c r="V13" s="80">
+        <f t="shared" si="2"/>
+        <v>-305</v>
+      </c>
+      <c r="W13" s="52">
+        <f t="shared" si="2"/>
+        <v>-311</v>
+      </c>
+      <c r="X13" s="56">
+        <f t="shared" si="2"/>
+        <v>-312</v>
+      </c>
+      <c r="Y13" s="117">
+        <f t="shared" si="2"/>
+        <v>-334</v>
+      </c>
+      <c r="Z13" s="80">
+        <f t="shared" si="2"/>
+        <v>-336</v>
+      </c>
+      <c r="AA13" s="52">
+        <f t="shared" si="2"/>
+        <v>-342</v>
+      </c>
+      <c r="AB13" s="65">
+        <f t="shared" si="4"/>
+        <v>-344</v>
+      </c>
+      <c r="AC13" s="119">
+        <f t="shared" si="3"/>
+        <v>-403</v>
+      </c>
+      <c r="AD13" s="80">
+        <f t="shared" si="3"/>
+        <v>-405</v>
+      </c>
+      <c r="AE13" s="58">
+        <f t="shared" si="3"/>
+        <v>-411</v>
+      </c>
+      <c r="AF13" s="56">
+        <f t="shared" si="3"/>
+        <v>-412</v>
+      </c>
+      <c r="AG13" s="119">
+        <f t="shared" si="3"/>
+        <v>-434</v>
+      </c>
+      <c r="AH13" s="80">
+        <f t="shared" si="3"/>
+        <v>-436</v>
+      </c>
+      <c r="AI13" s="58">
+        <f t="shared" si="3"/>
+        <v>-442</v>
+      </c>
+      <c r="AJ13" s="59">
+        <f t="shared" si="5"/>
+        <v>-444</v>
+      </c>
+      <c r="AK13">
+        <v>12</v>
+      </c>
+      <c r="AL13" s="30"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A14" s="7"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1045,40 +2954,181 @@
       <c r="Q14">
         <v>13</v>
       </c>
-      <c r="R14" s="27"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="22"/>
+      <c r="R14" s="30"/>
+      <c r="U14" s="45">
+        <f t="shared" si="2"/>
+        <v>-292</v>
+      </c>
+      <c r="V14" s="78">
+        <f t="shared" si="2"/>
+        <v>-294</v>
+      </c>
+      <c r="W14" s="51">
+        <f t="shared" si="2"/>
+        <v>-300</v>
+      </c>
+      <c r="X14" s="57">
+        <f t="shared" si="2"/>
+        <v>-302</v>
+      </c>
+      <c r="Y14" s="51">
+        <f t="shared" si="2"/>
+        <v>-323</v>
+      </c>
+      <c r="Z14" s="78">
+        <f t="shared" si="2"/>
+        <v>-325</v>
+      </c>
+      <c r="AA14" s="51">
+        <f t="shared" si="2"/>
+        <v>-331</v>
+      </c>
+      <c r="AB14" s="66">
+        <f t="shared" si="4"/>
+        <v>-333</v>
+      </c>
+      <c r="AC14" s="36">
+        <f t="shared" si="3"/>
+        <v>-392</v>
+      </c>
+      <c r="AD14" s="78">
+        <f t="shared" si="3"/>
+        <v>-394</v>
+      </c>
+      <c r="AE14" s="36">
+        <f t="shared" si="3"/>
+        <v>-400</v>
+      </c>
+      <c r="AF14" s="57">
+        <f t="shared" si="3"/>
+        <v>-402</v>
+      </c>
+      <c r="AG14" s="36">
+        <f t="shared" si="3"/>
+        <v>-423</v>
+      </c>
+      <c r="AH14" s="78">
+        <f t="shared" si="3"/>
+        <v>-425</v>
+      </c>
+      <c r="AI14" s="36">
+        <f t="shared" si="3"/>
+        <v>-431</v>
+      </c>
+      <c r="AJ14" s="37">
+        <f t="shared" si="5"/>
+        <v>-433</v>
+      </c>
+      <c r="AK14">
+        <v>13</v>
+      </c>
+      <c r="AL14" s="30"/>
     </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="7"/>
-      <c r="B15" s="1"/>
+    <row r="15" spans="1:40" ht="15.75" thickBot="1">
+      <c r="A15" s="19"/>
+      <c r="B15" s="123">
+        <v>5</v>
+      </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="123">
+        <v>5</v>
+      </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="123">
+        <v>5</v>
+      </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="122">
+        <v>5</v>
+      </c>
       <c r="I15" s="19"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="123">
+        <v>5</v>
+      </c>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="L15" s="123">
+        <v>5</v>
+      </c>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="N15" s="123">
+        <v>5</v>
+      </c>
       <c r="O15" s="1"/>
-      <c r="P15" s="8"/>
+      <c r="P15" s="122">
+        <v>5</v>
+      </c>
       <c r="Q15">
         <v>14</v>
       </c>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22"/>
-      <c r="Z15" s="22"/>
+      <c r="U15" s="86">
+        <f t="shared" si="2"/>
+        <v>-291</v>
+      </c>
+      <c r="V15" s="101">
+        <f t="shared" si="2"/>
+        <v>-293</v>
+      </c>
+      <c r="W15" s="88">
+        <f t="shared" si="2"/>
+        <v>-299</v>
+      </c>
+      <c r="X15" s="87">
+        <f t="shared" si="2"/>
+        <v>-301</v>
+      </c>
+      <c r="Y15" s="88">
+        <f t="shared" si="2"/>
+        <v>-322</v>
+      </c>
+      <c r="Z15" s="101">
+        <f t="shared" si="2"/>
+        <v>-324</v>
+      </c>
+      <c r="AA15" s="88">
+        <f t="shared" si="2"/>
+        <v>-330</v>
+      </c>
+      <c r="AB15" s="89">
+        <f t="shared" si="4"/>
+        <v>-332</v>
+      </c>
+      <c r="AC15" s="103">
+        <f t="shared" si="3"/>
+        <v>-391</v>
+      </c>
+      <c r="AD15" s="101">
+        <f t="shared" si="3"/>
+        <v>-393</v>
+      </c>
+      <c r="AE15" s="103">
+        <f t="shared" si="3"/>
+        <v>-399</v>
+      </c>
+      <c r="AF15" s="87">
+        <f t="shared" si="3"/>
+        <v>-401</v>
+      </c>
+      <c r="AG15" s="103">
+        <f t="shared" si="3"/>
+        <v>-422</v>
+      </c>
+      <c r="AH15" s="101">
+        <f t="shared" si="3"/>
+        <v>-424</v>
+      </c>
+      <c r="AI15" s="103">
+        <f t="shared" si="3"/>
+        <v>-430</v>
+      </c>
+      <c r="AJ15" s="104">
+        <f t="shared" si="5"/>
+        <v>-432</v>
+      </c>
+      <c r="AK15">
+        <v>14</v>
+      </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A16" s="7"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1098,59 +3148,191 @@
       <c r="Q16">
         <v>15</v>
       </c>
-      <c r="V16" s="22"/>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
+      <c r="U16" s="45">
+        <f t="shared" si="2"/>
+        <v>-288</v>
+      </c>
+      <c r="V16" s="78">
+        <f t="shared" si="2"/>
+        <v>-290</v>
+      </c>
+      <c r="W16" s="51">
+        <f t="shared" si="2"/>
+        <v>-296</v>
+      </c>
+      <c r="X16" s="57">
+        <f t="shared" si="2"/>
+        <v>-298</v>
+      </c>
+      <c r="Y16" s="51">
+        <f t="shared" si="2"/>
+        <v>-320</v>
+      </c>
+      <c r="Z16" s="78">
+        <f t="shared" si="2"/>
+        <v>-322</v>
+      </c>
+      <c r="AA16" s="51">
+        <f t="shared" si="2"/>
+        <v>-327</v>
+      </c>
+      <c r="AB16" s="66">
+        <f t="shared" si="4"/>
+        <v>-329</v>
+      </c>
+      <c r="AC16" s="36">
+        <f t="shared" si="3"/>
+        <v>-388</v>
+      </c>
+      <c r="AD16" s="78">
+        <f t="shared" si="3"/>
+        <v>-390</v>
+      </c>
+      <c r="AE16" s="36">
+        <f t="shared" si="3"/>
+        <v>-396</v>
+      </c>
+      <c r="AF16" s="57">
+        <f t="shared" si="3"/>
+        <v>-398</v>
+      </c>
+      <c r="AG16" s="36">
+        <f t="shared" si="3"/>
+        <v>-420</v>
+      </c>
+      <c r="AH16" s="78">
+        <f t="shared" si="3"/>
+        <v>-422</v>
+      </c>
+      <c r="AI16" s="36">
+        <f t="shared" si="3"/>
+        <v>-427</v>
+      </c>
+      <c r="AJ16" s="37">
+        <f t="shared" si="5"/>
+        <v>-429</v>
+      </c>
+      <c r="AK16">
+        <v>15</v>
+      </c>
     </row>
-    <row r="17" spans="1:26" ht="15" thickBot="1">
+    <row r="17" spans="1:37" ht="15.75" thickBot="1">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="C17" s="121">
+        <v>4</v>
+      </c>
       <c r="D17" s="10"/>
       <c r="E17" s="14">
         <v>2</v>
       </c>
       <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="G17" s="121">
+        <v>4</v>
+      </c>
       <c r="H17" s="16"/>
       <c r="I17" s="23">
         <v>0</v>
       </c>
       <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
+      <c r="K17" s="121">
+        <v>4</v>
+      </c>
       <c r="L17" s="10"/>
       <c r="M17" s="14">
         <v>2</v>
       </c>
       <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
+      <c r="O17" s="121">
+        <v>4</v>
+      </c>
       <c r="P17" s="11"/>
       <c r="Q17">
         <v>16</v>
       </c>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
-      <c r="Z17" s="22"/>
+      <c r="U17" s="27">
+        <f t="shared" si="2"/>
+        <v>-287</v>
+      </c>
+      <c r="V17" s="79">
+        <f t="shared" si="2"/>
+        <v>-289</v>
+      </c>
+      <c r="W17" s="50">
+        <f t="shared" si="2"/>
+        <v>-295</v>
+      </c>
+      <c r="X17" s="55">
+        <f t="shared" si="2"/>
+        <v>-297</v>
+      </c>
+      <c r="Y17" s="114">
+        <f t="shared" si="2"/>
+        <v>-319</v>
+      </c>
+      <c r="Z17" s="79">
+        <f t="shared" si="2"/>
+        <v>-321</v>
+      </c>
+      <c r="AA17" s="50">
+        <f t="shared" si="2"/>
+        <v>-326</v>
+      </c>
+      <c r="AB17" s="64">
+        <f t="shared" si="4"/>
+        <v>-328</v>
+      </c>
+      <c r="AC17" s="111">
+        <f t="shared" si="3"/>
+        <v>-387</v>
+      </c>
+      <c r="AD17" s="79">
+        <f t="shared" si="3"/>
+        <v>-389</v>
+      </c>
+      <c r="AE17" s="34">
+        <f t="shared" si="3"/>
+        <v>-395</v>
+      </c>
+      <c r="AF17" s="55">
+        <f t="shared" si="3"/>
+        <v>-397</v>
+      </c>
+      <c r="AG17" s="115">
+        <f t="shared" si="3"/>
+        <v>-419</v>
+      </c>
+      <c r="AH17" s="79">
+        <f t="shared" si="3"/>
+        <v>-421</v>
+      </c>
+      <c r="AI17" s="34">
+        <f t="shared" si="3"/>
+        <v>-426</v>
+      </c>
+      <c r="AJ17" s="29">
+        <f t="shared" si="5"/>
+        <v>-428</v>
+      </c>
+      <c r="AK17">
+        <v>16</v>
+      </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:37">
       <c r="V18" s="22"/>
       <c r="W18" s="22"/>
       <c r="X18" s="22"/>
       <c r="Y18" s="22"/>
       <c r="Z18" s="22"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:37">
       <c r="V19" s="22"/>
       <c r="W19" s="22"/>
       <c r="X19" s="22"/>
       <c r="Y19" s="22"/>
       <c r="Z19" s="22"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:37">
       <c r="V20" s="22"/>
       <c r="W20" s="22"/>
       <c r="X20" s="22"/>
@@ -1158,8 +3340,9 @@
       <c r="Z20" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="R8:R14"/>
+    <mergeCell ref="AL8:AL14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1168,11 +3351,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1180,11 +3364,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Matrix search (ex5.) forward working solution.
</commit_message>
<xml_diff>
--- a/20441/maman16/Drawing.xlsx
+++ b/20441/maman16/Drawing.xlsx
@@ -15,6 +15,184 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Maxim Veksler</author>
+  </authors>
+  <commentList>
+    <comment ref="U9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t>Maxim Veksler:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t xml:space="preserve">
+n=16</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t>Maxim Veksler:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t xml:space="preserve">
+n=8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t>Maxim Veksler:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t xml:space="preserve">
+n=16</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t>Maxim Veksler:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t xml:space="preserve">
+n=8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t>Maxim Veksler:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t xml:space="preserve">
+n=8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t>Maxim Veksler:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t xml:space="preserve">
+n=16</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t>Maxim Veksler:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="177"/>
+          </rPr>
+          <t xml:space="preserve">
+n=8</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
@@ -25,7 +203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,6 +215,26 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="177"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="177"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
@@ -106,7 +304,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1113,7 +1311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1158,9 +1356,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -1196,12 +1391,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -1214,9 +1403,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -1229,9 +1415,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -1244,19 +1427,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1402,14 +1576,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1708,7 +1915,7 @@
   <dimension ref="A1:AN20"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
@@ -1792,7 +1999,7 @@
       <c r="AA1" s="3">
         <v>10</v>
       </c>
-      <c r="AB1" s="35">
+      <c r="AB1" s="34">
         <v>9</v>
       </c>
       <c r="AC1" s="32">
@@ -1844,53 +2051,53 @@
         <f t="shared" ref="U2:AA9" si="0">AC2+100</f>
         <v>-358</v>
       </c>
-      <c r="V2" s="79">
+      <c r="V2" s="71">
         <f t="shared" si="0"/>
         <v>-360</v>
       </c>
-      <c r="W2" s="50">
+      <c r="W2" s="49">
         <f t="shared" si="0"/>
         <v>-366</v>
       </c>
-      <c r="X2" s="55">
+      <c r="X2" s="52">
         <f t="shared" si="0"/>
         <v>-368</v>
       </c>
-      <c r="Y2" s="50">
+      <c r="Y2" s="49">
         <f t="shared" si="0"/>
         <v>-389</v>
       </c>
-      <c r="Z2" s="79">
+      <c r="Z2" s="71">
         <f t="shared" si="0"/>
         <v>-391</v>
       </c>
-      <c r="AA2" s="50">
+      <c r="AA2" s="49">
         <f t="shared" si="0"/>
         <v>-398</v>
       </c>
-      <c r="AB2" s="64">
+      <c r="AB2" s="59">
         <f>AJ2+100</f>
         <v>-400</v>
       </c>
       <c r="AC2" s="33">
         <v>-458</v>
       </c>
-      <c r="AD2" s="95">
+      <c r="AD2" s="87">
         <v>-460</v>
       </c>
       <c r="AE2" s="33">
         <v>-466</v>
       </c>
-      <c r="AF2" s="60">
+      <c r="AF2" s="56">
         <v>-468</v>
       </c>
-      <c r="AG2" s="46">
+      <c r="AG2" s="45">
         <v>-489</v>
       </c>
-      <c r="AH2" s="74">
+      <c r="AH2" s="66">
         <v>-491</v>
       </c>
-      <c r="AI2" s="46">
+      <c r="AI2" s="45">
         <v>-498</v>
       </c>
       <c r="AJ2" s="28">
@@ -1901,95 +2108,79 @@
       </c>
     </row>
     <row r="3" spans="1:40" ht="15.75" thickBot="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="123">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="123">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="123">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="122">
-        <v>5</v>
-      </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="123">
-        <v>5</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="123">
-        <v>5</v>
-      </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="123">
-        <v>5</v>
-      </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="122">
-        <v>5</v>
-      </c>
+      <c r="A3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
+      <c r="N3" s="124"/>
+      <c r="O3" s="124"/>
+      <c r="P3" s="125"/>
       <c r="Q3">
         <v>2</v>
       </c>
-      <c r="U3" s="86">
+      <c r="U3" s="78">
         <f t="shared" si="0"/>
         <v>-357</v>
       </c>
-      <c r="V3" s="101">
+      <c r="V3" s="93">
         <f t="shared" si="0"/>
         <v>-359</v>
       </c>
-      <c r="W3" s="88">
+      <c r="W3" s="80">
         <f t="shared" si="0"/>
         <v>-365</v>
       </c>
-      <c r="X3" s="87">
+      <c r="X3" s="79">
         <f t="shared" si="0"/>
         <v>-367</v>
       </c>
-      <c r="Y3" s="88">
+      <c r="Y3" s="80">
         <f t="shared" si="0"/>
         <v>-388</v>
       </c>
-      <c r="Z3" s="101">
+      <c r="Z3" s="93">
         <f t="shared" si="0"/>
         <v>-390</v>
       </c>
-      <c r="AA3" s="88">
+      <c r="AA3" s="80">
         <f t="shared" si="0"/>
         <v>-397</v>
       </c>
-      <c r="AB3" s="89">
+      <c r="AB3" s="81">
         <f t="shared" ref="AB3:AB9" si="1">AJ3+100</f>
         <v>-399</v>
       </c>
-      <c r="AC3" s="90">
+      <c r="AC3" s="82">
         <v>-457</v>
       </c>
-      <c r="AD3" s="96">
+      <c r="AD3" s="88">
         <v>-459</v>
       </c>
-      <c r="AE3" s="90">
+      <c r="AE3" s="82">
         <v>-465</v>
       </c>
-      <c r="AF3" s="91">
+      <c r="AF3" s="83">
         <v>-467</v>
       </c>
-      <c r="AG3" s="92">
+      <c r="AG3" s="84">
         <v>-488</v>
       </c>
-      <c r="AH3" s="93">
+      <c r="AH3" s="85">
         <v>-490</v>
       </c>
-      <c r="AI3" s="92">
+      <c r="AI3" s="84">
         <v>-497</v>
       </c>
-      <c r="AJ3" s="94">
+      <c r="AJ3" s="86">
         <v>-499</v>
       </c>
       <c r="AK3">
@@ -2016,73 +2207,73 @@
       <c r="Q4">
         <v>3</v>
       </c>
-      <c r="U4" s="45">
+      <c r="U4" s="44">
         <f t="shared" si="0"/>
         <v>-354</v>
       </c>
-      <c r="V4" s="78">
+      <c r="V4" s="70">
         <f t="shared" si="0"/>
         <v>-356</v>
       </c>
-      <c r="W4" s="51">
+      <c r="W4" s="50">
         <f t="shared" si="0"/>
         <v>-363</v>
       </c>
-      <c r="X4" s="57">
+      <c r="X4" s="54">
         <f t="shared" si="0"/>
         <v>-364</v>
       </c>
-      <c r="Y4" s="51">
+      <c r="Y4" s="50">
         <f t="shared" si="0"/>
         <v>-385</v>
       </c>
-      <c r="Z4" s="78">
+      <c r="Z4" s="70">
         <f t="shared" si="0"/>
         <v>-387</v>
       </c>
-      <c r="AA4" s="51">
+      <c r="AA4" s="50">
         <f t="shared" si="0"/>
         <v>-393</v>
       </c>
-      <c r="AB4" s="66">
+      <c r="AB4" s="61">
         <f t="shared" si="1"/>
         <v>-395</v>
       </c>
-      <c r="AC4" s="81">
+      <c r="AC4" s="73">
         <v>-454</v>
       </c>
-      <c r="AD4" s="97">
+      <c r="AD4" s="89">
         <v>-456</v>
       </c>
-      <c r="AE4" s="81">
+      <c r="AE4" s="73">
         <v>-463</v>
       </c>
-      <c r="AF4" s="82">
+      <c r="AF4" s="74">
         <v>-464</v>
       </c>
-      <c r="AG4" s="83">
+      <c r="AG4" s="75">
         <v>-485</v>
       </c>
-      <c r="AH4" s="84">
+      <c r="AH4" s="76">
         <v>-487</v>
       </c>
-      <c r="AI4" s="83">
+      <c r="AI4" s="75">
         <v>-493</v>
       </c>
-      <c r="AJ4" s="85">
+      <c r="AJ4" s="77">
         <v>-495</v>
       </c>
       <c r="AK4">
         <v>3</v>
       </c>
-      <c r="AM4" s="44"/>
+      <c r="AM4" s="43"/>
     </row>
     <row r="5" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="26">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="120">
+      <c r="C5" s="112">
         <v>4</v>
       </c>
       <c r="D5" s="1"/>
@@ -2090,7 +2281,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="120">
+      <c r="G5" s="112">
         <v>4</v>
       </c>
       <c r="H5" s="2"/>
@@ -2098,7 +2289,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="120">
+      <c r="K5" s="112">
         <v>4</v>
       </c>
       <c r="L5" s="1"/>
@@ -2106,75 +2297,75 @@
         <v>3</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="120">
+      <c r="O5" s="112">
         <v>4</v>
       </c>
       <c r="P5" s="8"/>
       <c r="Q5">
         <v>4</v>
       </c>
-      <c r="U5" s="118">
+      <c r="U5" s="110">
         <f t="shared" si="0"/>
         <v>-353</v>
       </c>
-      <c r="V5" s="80">
+      <c r="V5" s="72">
         <f t="shared" si="0"/>
         <v>-355</v>
       </c>
-      <c r="W5" s="52">
+      <c r="W5" s="116">
         <f t="shared" si="0"/>
         <v>-361</v>
       </c>
-      <c r="X5" s="56">
+      <c r="X5" s="53">
         <f t="shared" si="0"/>
         <v>-362</v>
       </c>
-      <c r="Y5" s="117">
+      <c r="Y5" s="109">
         <f t="shared" si="0"/>
         <v>-384</v>
       </c>
-      <c r="Z5" s="80">
+      <c r="Z5" s="72">
         <f t="shared" si="0"/>
         <v>-386</v>
       </c>
-      <c r="AA5" s="52">
+      <c r="AA5" s="116">
         <f t="shared" si="0"/>
         <v>-392</v>
       </c>
-      <c r="AB5" s="65">
+      <c r="AB5" s="60">
         <f t="shared" si="1"/>
         <v>-394</v>
       </c>
-      <c r="AC5" s="116">
+      <c r="AC5" s="108">
         <v>-453</v>
       </c>
-      <c r="AD5" s="98">
+      <c r="AD5" s="90">
         <v>-455</v>
       </c>
-      <c r="AE5" s="63">
+      <c r="AE5" s="119">
         <v>-461</v>
       </c>
-      <c r="AF5" s="61">
+      <c r="AF5" s="57">
         <v>-462</v>
       </c>
-      <c r="AG5" s="116">
+      <c r="AG5" s="108">
         <v>-484</v>
       </c>
-      <c r="AH5" s="75">
+      <c r="AH5" s="67">
         <v>-486</v>
       </c>
-      <c r="AI5" s="53">
+      <c r="AI5" s="119">
         <v>-492</v>
       </c>
-      <c r="AJ5" s="54">
+      <c r="AJ5" s="51">
         <v>-494</v>
       </c>
       <c r="AK5">
         <v>4</v>
       </c>
-      <c r="AL5" s="43"/>
-      <c r="AM5" s="38"/>
-      <c r="AN5" s="39"/>
+      <c r="AL5" s="42"/>
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="38"/>
     </row>
     <row r="6" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A6" s="7"/>
@@ -2196,165 +2387,149 @@
       <c r="Q6">
         <v>5</v>
       </c>
-      <c r="U6" s="45">
+      <c r="U6" s="44">
         <f t="shared" si="0"/>
         <v>-342</v>
       </c>
-      <c r="V6" s="78">
+      <c r="V6" s="70">
         <f t="shared" si="0"/>
         <v>-344</v>
       </c>
-      <c r="W6" s="51">
+      <c r="W6" s="50">
         <f t="shared" si="0"/>
         <v>-350</v>
       </c>
-      <c r="X6" s="57">
+      <c r="X6" s="54">
         <f t="shared" si="0"/>
         <v>-352</v>
       </c>
-      <c r="Y6" s="51">
+      <c r="Y6" s="50">
         <f t="shared" si="0"/>
         <v>-373</v>
       </c>
-      <c r="Z6" s="78">
+      <c r="Z6" s="70">
         <f t="shared" si="0"/>
         <v>-375</v>
       </c>
-      <c r="AA6" s="51">
+      <c r="AA6" s="50">
         <f t="shared" si="0"/>
         <v>-381</v>
       </c>
-      <c r="AB6" s="66">
+      <c r="AB6" s="61">
         <f t="shared" si="1"/>
         <v>-383</v>
       </c>
-      <c r="AC6" s="47">
+      <c r="AC6" s="46">
         <v>-442</v>
       </c>
-      <c r="AD6" s="99">
+      <c r="AD6" s="91">
         <v>-444</v>
       </c>
-      <c r="AE6" s="47">
+      <c r="AE6" s="46">
         <v>-450</v>
       </c>
-      <c r="AF6" s="62">
+      <c r="AF6" s="58">
         <v>-452</v>
       </c>
-      <c r="AG6" s="48">
+      <c r="AG6" s="47">
         <v>-473</v>
       </c>
-      <c r="AH6" s="76">
+      <c r="AH6" s="68">
         <v>-475</v>
       </c>
-      <c r="AI6" s="48">
+      <c r="AI6" s="47">
         <v>-481</v>
       </c>
-      <c r="AJ6" s="49">
+      <c r="AJ6" s="48">
         <v>-483</v>
       </c>
       <c r="AK6">
         <v>5</v>
       </c>
       <c r="AM6" s="21"/>
-      <c r="AN6" s="40"/>
+      <c r="AN6" s="39"/>
     </row>
     <row r="7" spans="1:40" ht="15.75" thickBot="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="123">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="123">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="123">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="122">
-        <v>5</v>
-      </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="123">
-        <v>5</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="123">
-        <v>5</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="123">
-        <v>5</v>
-      </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="122">
-        <v>5</v>
-      </c>
+      <c r="A7" s="123"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
+      <c r="O7" s="124"/>
+      <c r="P7" s="125"/>
       <c r="Q7">
         <v>6</v>
       </c>
-      <c r="U7" s="86">
+      <c r="U7" s="78">
         <f t="shared" si="0"/>
         <v>-341</v>
       </c>
-      <c r="V7" s="101">
+      <c r="V7" s="93">
         <f t="shared" si="0"/>
         <v>-343</v>
       </c>
-      <c r="W7" s="88">
+      <c r="W7" s="80">
         <f t="shared" si="0"/>
         <v>-349</v>
       </c>
-      <c r="X7" s="87">
+      <c r="X7" s="79">
         <f t="shared" si="0"/>
         <v>-351</v>
       </c>
-      <c r="Y7" s="88">
+      <c r="Y7" s="80">
         <f t="shared" si="0"/>
         <v>-372</v>
       </c>
-      <c r="Z7" s="101">
+      <c r="Z7" s="93">
         <f t="shared" si="0"/>
         <v>-374</v>
       </c>
-      <c r="AA7" s="88">
+      <c r="AA7" s="80">
         <f t="shared" si="0"/>
         <v>-380</v>
       </c>
-      <c r="AB7" s="89">
+      <c r="AB7" s="81">
         <f t="shared" si="1"/>
         <v>-382</v>
       </c>
-      <c r="AC7" s="105">
+      <c r="AC7" s="97">
         <v>-441</v>
       </c>
-      <c r="AD7" s="106">
+      <c r="AD7" s="98">
         <v>-443</v>
       </c>
-      <c r="AE7" s="105">
+      <c r="AE7" s="97">
         <v>-449</v>
       </c>
-      <c r="AF7" s="107">
+      <c r="AF7" s="99">
         <v>-451</v>
       </c>
-      <c r="AG7" s="108">
+      <c r="AG7" s="100">
         <v>-472</v>
       </c>
-      <c r="AH7" s="109">
+      <c r="AH7" s="101">
         <v>-474</v>
       </c>
-      <c r="AI7" s="108">
+      <c r="AI7" s="100">
         <v>-480</v>
       </c>
-      <c r="AJ7" s="110">
+      <c r="AJ7" s="102">
         <v>-482</v>
       </c>
       <c r="AK7">
         <v>6</v>
       </c>
       <c r="AM7" s="21"/>
-      <c r="AN7" s="40"/>
+      <c r="AN7" s="39"/>
     </row>
     <row r="8" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A8" s="7"/>
@@ -2379,60 +2554,60 @@
       <c r="R8" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="U8" s="45">
+      <c r="U8" s="44">
         <f t="shared" si="0"/>
         <v>-338</v>
       </c>
-      <c r="V8" s="78">
+      <c r="V8" s="70">
         <f t="shared" si="0"/>
         <v>-340</v>
       </c>
-      <c r="W8" s="51">
+      <c r="W8" s="50">
         <f t="shared" si="0"/>
         <v>-346</v>
       </c>
-      <c r="X8" s="57">
+      <c r="X8" s="54">
         <f t="shared" si="0"/>
         <v>-348</v>
       </c>
-      <c r="Y8" s="51">
+      <c r="Y8" s="50">
         <f t="shared" si="0"/>
         <v>-370</v>
       </c>
-      <c r="Z8" s="78">
+      <c r="Z8" s="70">
         <f t="shared" si="0"/>
         <v>-372</v>
       </c>
-      <c r="AA8" s="51">
+      <c r="AA8" s="50">
         <f t="shared" si="0"/>
         <v>-377</v>
       </c>
-      <c r="AB8" s="66">
+      <c r="AB8" s="61">
         <f t="shared" si="1"/>
         <v>-379</v>
       </c>
-      <c r="AC8" s="47">
+      <c r="AC8" s="46">
         <v>-438</v>
       </c>
-      <c r="AD8" s="99">
+      <c r="AD8" s="91">
         <v>-440</v>
       </c>
-      <c r="AE8" s="47">
+      <c r="AE8" s="46">
         <v>-446</v>
       </c>
-      <c r="AF8" s="62">
+      <c r="AF8" s="58">
         <v>-448</v>
       </c>
-      <c r="AG8" s="48">
+      <c r="AG8" s="47">
         <v>-470</v>
       </c>
-      <c r="AH8" s="76">
+      <c r="AH8" s="68">
         <v>-472</v>
       </c>
-      <c r="AI8" s="48">
+      <c r="AI8" s="47">
         <v>-477</v>
       </c>
-      <c r="AJ8" s="49">
+      <c r="AJ8" s="48">
         <v>-479</v>
       </c>
       <c r="AK8">
@@ -2441,15 +2616,15 @@
       <c r="AL8" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="AM8" s="41"/>
-      <c r="AN8" s="42"/>
+      <c r="AM8" s="40"/>
+      <c r="AN8" s="41"/>
     </row>
     <row r="9" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
       <c r="A9" s="13">
         <v>1</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="121">
+      <c r="C9" s="113">
         <v>4</v>
       </c>
       <c r="D9" s="10"/>
@@ -2457,7 +2632,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="121">
+      <c r="G9" s="113">
         <v>4</v>
       </c>
       <c r="H9" s="16"/>
@@ -2465,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="120">
+      <c r="K9" s="112">
         <v>4</v>
       </c>
       <c r="L9" s="10"/>
@@ -2473,7 +2648,7 @@
         <v>2</v>
       </c>
       <c r="N9" s="10"/>
-      <c r="O9" s="121">
+      <c r="O9" s="132">
         <v>4</v>
       </c>
       <c r="P9" s="11"/>
@@ -2481,60 +2656,60 @@
         <v>8</v>
       </c>
       <c r="R9" s="30"/>
-      <c r="U9" s="125">
+      <c r="U9" s="115">
         <f t="shared" si="0"/>
         <v>-337</v>
       </c>
-      <c r="V9" s="102">
+      <c r="V9" s="94">
         <f t="shared" si="0"/>
         <v>-339</v>
       </c>
-      <c r="W9" s="68">
+      <c r="W9" s="118">
         <f t="shared" si="0"/>
         <v>-345</v>
       </c>
-      <c r="X9" s="67">
+      <c r="X9" s="62">
         <f t="shared" si="0"/>
         <v>-347</v>
       </c>
-      <c r="Y9" s="113">
+      <c r="Y9" s="105">
         <f t="shared" si="0"/>
         <v>-369</v>
       </c>
-      <c r="Z9" s="102">
+      <c r="Z9" s="94">
         <f t="shared" si="0"/>
         <v>-371</v>
       </c>
-      <c r="AA9" s="68">
+      <c r="AA9" s="118">
         <f t="shared" si="0"/>
         <v>-376</v>
       </c>
-      <c r="AB9" s="69">
+      <c r="AB9" s="63">
         <f t="shared" si="1"/>
         <v>-378</v>
       </c>
-      <c r="AC9" s="124">
+      <c r="AC9" s="114">
         <v>-437</v>
       </c>
-      <c r="AD9" s="100">
+      <c r="AD9" s="92">
         <v>-439</v>
       </c>
-      <c r="AE9" s="70">
+      <c r="AE9" s="120">
         <v>-445</v>
       </c>
-      <c r="AF9" s="71">
+      <c r="AF9" s="64">
         <v>-447</v>
       </c>
-      <c r="AG9" s="112">
+      <c r="AG9" s="104">
         <v>-469</v>
       </c>
-      <c r="AH9" s="77">
+      <c r="AH9" s="69">
         <v>-471</v>
       </c>
-      <c r="AI9" s="72">
+      <c r="AI9" s="120">
         <v>-476</v>
       </c>
-      <c r="AJ9" s="73">
+      <c r="AJ9" s="65">
         <v>-478</v>
       </c>
       <c r="AK9">
@@ -2563,67 +2738,67 @@
         <v>9</v>
       </c>
       <c r="R10" s="30"/>
-      <c r="U10" s="45">
+      <c r="U10" s="44">
         <f t="shared" ref="U10:AA17" si="2">AC2+150</f>
         <v>-308</v>
       </c>
-      <c r="V10" s="78">
+      <c r="V10" s="70">
         <f t="shared" si="2"/>
         <v>-310</v>
       </c>
-      <c r="W10" s="51">
+      <c r="W10" s="50">
         <f t="shared" si="2"/>
         <v>-316</v>
       </c>
-      <c r="X10" s="57">
+      <c r="X10" s="54">
         <f t="shared" si="2"/>
         <v>-318</v>
       </c>
-      <c r="Y10" s="51">
+      <c r="Y10" s="50">
         <f t="shared" si="2"/>
         <v>-339</v>
       </c>
-      <c r="Z10" s="78">
+      <c r="Z10" s="70">
         <f t="shared" si="2"/>
         <v>-341</v>
       </c>
-      <c r="AA10" s="51">
+      <c r="AA10" s="50">
         <f t="shared" si="2"/>
         <v>-348</v>
       </c>
-      <c r="AB10" s="66">
+      <c r="AB10" s="61">
         <f>AJ2+150</f>
         <v>-350</v>
       </c>
-      <c r="AC10" s="36">
+      <c r="AC10" s="35">
         <f t="shared" ref="AC10:AI17" si="3">AC2+50</f>
         <v>-408</v>
       </c>
-      <c r="AD10" s="78">
+      <c r="AD10" s="70">
         <f t="shared" si="3"/>
         <v>-410</v>
       </c>
-      <c r="AE10" s="36">
+      <c r="AE10" s="35">
         <f t="shared" si="3"/>
         <v>-416</v>
       </c>
-      <c r="AF10" s="57">
+      <c r="AF10" s="54">
         <f t="shared" si="3"/>
         <v>-418</v>
       </c>
-      <c r="AG10" s="36">
+      <c r="AG10" s="35">
         <f t="shared" si="3"/>
         <v>-439</v>
       </c>
-      <c r="AH10" s="78">
+      <c r="AH10" s="70">
         <f t="shared" si="3"/>
         <v>-441</v>
       </c>
-      <c r="AI10" s="36">
+      <c r="AI10" s="35">
         <f t="shared" si="3"/>
         <v>-448</v>
       </c>
-      <c r="AJ10" s="37">
+      <c r="AJ10" s="36">
         <f>AJ2+50</f>
         <v>-450</v>
       </c>
@@ -2633,103 +2808,87 @@
       <c r="AL10" s="30"/>
     </row>
     <row r="11" spans="1:40" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A11" s="19"/>
-      <c r="B11" s="123">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="123">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="123">
-        <v>5</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="122">
-        <v>5</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="123">
-        <v>5</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="123">
-        <v>5</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="123">
-        <v>5</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="122">
-        <v>5</v>
-      </c>
+      <c r="A11" s="123"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="124"/>
+      <c r="D11" s="124"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="124"/>
+      <c r="O11" s="124"/>
+      <c r="P11" s="125"/>
       <c r="Q11">
         <v>10</v>
       </c>
       <c r="R11" s="30"/>
-      <c r="U11" s="86">
+      <c r="U11" s="78">
         <f t="shared" si="2"/>
         <v>-307</v>
       </c>
-      <c r="V11" s="101">
+      <c r="V11" s="93">
         <f t="shared" si="2"/>
         <v>-309</v>
       </c>
-      <c r="W11" s="88">
+      <c r="W11" s="80">
         <f t="shared" si="2"/>
         <v>-315</v>
       </c>
-      <c r="X11" s="87">
+      <c r="X11" s="79">
         <f t="shared" si="2"/>
         <v>-317</v>
       </c>
-      <c r="Y11" s="88">
+      <c r="Y11" s="80">
         <f t="shared" si="2"/>
         <v>-338</v>
       </c>
-      <c r="Z11" s="101">
+      <c r="Z11" s="93">
         <f t="shared" si="2"/>
         <v>-340</v>
       </c>
-      <c r="AA11" s="88">
+      <c r="AA11" s="80">
         <f t="shared" si="2"/>
         <v>-347</v>
       </c>
-      <c r="AB11" s="89">
+      <c r="AB11" s="81">
         <f t="shared" ref="AB11:AB17" si="4">AJ3+150</f>
         <v>-349</v>
       </c>
-      <c r="AC11" s="103">
+      <c r="AC11" s="95">
         <f t="shared" si="3"/>
         <v>-407</v>
       </c>
-      <c r="AD11" s="101">
+      <c r="AD11" s="93">
         <f t="shared" si="3"/>
         <v>-409</v>
       </c>
-      <c r="AE11" s="103">
+      <c r="AE11" s="95">
         <f t="shared" si="3"/>
         <v>-415</v>
       </c>
-      <c r="AF11" s="87">
+      <c r="AF11" s="79">
         <f t="shared" si="3"/>
         <v>-417</v>
       </c>
-      <c r="AG11" s="103">
+      <c r="AG11" s="95">
         <f t="shared" si="3"/>
         <v>-438</v>
       </c>
-      <c r="AH11" s="101">
+      <c r="AH11" s="93">
         <f t="shared" si="3"/>
         <v>-440</v>
       </c>
-      <c r="AI11" s="103">
+      <c r="AI11" s="95">
         <f t="shared" si="3"/>
         <v>-447</v>
       </c>
-      <c r="AJ11" s="104">
+      <c r="AJ11" s="96">
         <f t="shared" ref="AJ11:AJ17" si="5">AJ3+50</f>
         <v>-449</v>
       </c>
@@ -2759,67 +2918,67 @@
         <v>11</v>
       </c>
       <c r="R12" s="30"/>
-      <c r="U12" s="45">
+      <c r="U12" s="44">
         <f t="shared" si="2"/>
         <v>-304</v>
       </c>
-      <c r="V12" s="78">
+      <c r="V12" s="70">
         <f t="shared" si="2"/>
         <v>-306</v>
       </c>
-      <c r="W12" s="51">
+      <c r="W12" s="50">
         <f t="shared" si="2"/>
         <v>-313</v>
       </c>
-      <c r="X12" s="57">
+      <c r="X12" s="54">
         <f t="shared" si="2"/>
         <v>-314</v>
       </c>
-      <c r="Y12" s="51">
+      <c r="Y12" s="50">
         <f t="shared" si="2"/>
         <v>-335</v>
       </c>
-      <c r="Z12" s="78">
+      <c r="Z12" s="70">
         <f t="shared" si="2"/>
         <v>-337</v>
       </c>
-      <c r="AA12" s="51">
+      <c r="AA12" s="50">
         <f t="shared" si="2"/>
         <v>-343</v>
       </c>
-      <c r="AB12" s="66">
+      <c r="AB12" s="61">
         <f t="shared" si="4"/>
         <v>-345</v>
       </c>
-      <c r="AC12" s="36">
+      <c r="AC12" s="35">
         <f t="shared" si="3"/>
         <v>-404</v>
       </c>
-      <c r="AD12" s="78">
+      <c r="AD12" s="70">
         <f t="shared" si="3"/>
         <v>-406</v>
       </c>
-      <c r="AE12" s="36">
+      <c r="AE12" s="35">
         <f t="shared" si="3"/>
         <v>-413</v>
       </c>
-      <c r="AF12" s="57">
+      <c r="AF12" s="54">
         <f t="shared" si="3"/>
         <v>-414</v>
       </c>
-      <c r="AG12" s="36">
+      <c r="AG12" s="35">
         <f t="shared" si="3"/>
         <v>-435</v>
       </c>
-      <c r="AH12" s="78">
+      <c r="AH12" s="70">
         <f t="shared" si="3"/>
         <v>-437</v>
       </c>
-      <c r="AI12" s="36">
+      <c r="AI12" s="35">
         <f t="shared" si="3"/>
         <v>-443</v>
       </c>
-      <c r="AJ12" s="37">
+      <c r="AJ12" s="36">
         <f t="shared" si="5"/>
         <v>-445</v>
       </c>
@@ -2833,7 +2992,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="120">
+      <c r="C13" s="112">
         <v>4</v>
       </c>
       <c r="D13" s="1"/>
@@ -2841,7 +3000,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="120">
+      <c r="G13" s="112">
         <v>4</v>
       </c>
       <c r="H13" s="2"/>
@@ -2849,7 +3008,7 @@
         <v>3</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="120">
+      <c r="K13" s="112">
         <v>4</v>
       </c>
       <c r="L13" s="1"/>
@@ -2857,7 +3016,7 @@
         <v>3</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="120">
+      <c r="O13" s="112">
         <v>4</v>
       </c>
       <c r="P13" s="8"/>
@@ -2865,67 +3024,67 @@
         <v>12</v>
       </c>
       <c r="R13" s="30"/>
-      <c r="U13" s="118">
+      <c r="U13" s="110">
         <f t="shared" si="2"/>
         <v>-303</v>
       </c>
-      <c r="V13" s="80">
+      <c r="V13" s="72">
         <f t="shared" si="2"/>
         <v>-305</v>
       </c>
-      <c r="W13" s="52">
+      <c r="W13" s="116">
         <f t="shared" si="2"/>
         <v>-311</v>
       </c>
-      <c r="X13" s="56">
+      <c r="X13" s="53">
         <f t="shared" si="2"/>
         <v>-312</v>
       </c>
-      <c r="Y13" s="117">
+      <c r="Y13" s="109">
         <f t="shared" si="2"/>
         <v>-334</v>
       </c>
-      <c r="Z13" s="80">
+      <c r="Z13" s="72">
         <f t="shared" si="2"/>
         <v>-336</v>
       </c>
-      <c r="AA13" s="52">
+      <c r="AA13" s="116">
         <f t="shared" si="2"/>
         <v>-342</v>
       </c>
-      <c r="AB13" s="65">
+      <c r="AB13" s="60">
         <f t="shared" si="4"/>
         <v>-344</v>
       </c>
-      <c r="AC13" s="119">
+      <c r="AC13" s="111">
         <f t="shared" si="3"/>
         <v>-403</v>
       </c>
-      <c r="AD13" s="80">
+      <c r="AD13" s="72">
         <f t="shared" si="3"/>
         <v>-405</v>
       </c>
-      <c r="AE13" s="58">
+      <c r="AE13" s="121">
         <f t="shared" si="3"/>
         <v>-411</v>
       </c>
-      <c r="AF13" s="56">
+      <c r="AF13" s="53">
         <f t="shared" si="3"/>
         <v>-412</v>
       </c>
-      <c r="AG13" s="119">
+      <c r="AG13" s="111">
         <f t="shared" si="3"/>
         <v>-434</v>
       </c>
-      <c r="AH13" s="80">
+      <c r="AH13" s="72">
         <f t="shared" si="3"/>
         <v>-436</v>
       </c>
-      <c r="AI13" s="58">
+      <c r="AI13" s="121">
         <f t="shared" si="3"/>
         <v>-442</v>
       </c>
-      <c r="AJ13" s="59">
+      <c r="AJ13" s="55">
         <f t="shared" si="5"/>
         <v>-444</v>
       </c>
@@ -2935,87 +3094,87 @@
       <c r="AL13" s="30"/>
     </row>
     <row r="14" spans="1:40" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="8"/>
+      <c r="A14" s="126"/>
+      <c r="B14" s="124"/>
+      <c r="C14" s="124"/>
+      <c r="D14" s="124"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="124"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="124"/>
+      <c r="P14" s="125"/>
       <c r="Q14">
         <v>13</v>
       </c>
       <c r="R14" s="30"/>
-      <c r="U14" s="45">
+      <c r="U14" s="44">
         <f t="shared" si="2"/>
         <v>-292</v>
       </c>
-      <c r="V14" s="78">
+      <c r="V14" s="70">
         <f t="shared" si="2"/>
         <v>-294</v>
       </c>
-      <c r="W14" s="51">
+      <c r="W14" s="50">
         <f t="shared" si="2"/>
         <v>-300</v>
       </c>
-      <c r="X14" s="57">
+      <c r="X14" s="54">
         <f t="shared" si="2"/>
         <v>-302</v>
       </c>
-      <c r="Y14" s="51">
+      <c r="Y14" s="50">
         <f t="shared" si="2"/>
         <v>-323</v>
       </c>
-      <c r="Z14" s="78">
+      <c r="Z14" s="70">
         <f t="shared" si="2"/>
         <v>-325</v>
       </c>
-      <c r="AA14" s="51">
+      <c r="AA14" s="50">
         <f t="shared" si="2"/>
         <v>-331</v>
       </c>
-      <c r="AB14" s="66">
+      <c r="AB14" s="61">
         <f t="shared" si="4"/>
         <v>-333</v>
       </c>
-      <c r="AC14" s="36">
+      <c r="AC14" s="35">
         <f t="shared" si="3"/>
         <v>-392</v>
       </c>
-      <c r="AD14" s="78">
+      <c r="AD14" s="70">
         <f t="shared" si="3"/>
         <v>-394</v>
       </c>
-      <c r="AE14" s="36">
+      <c r="AE14" s="35">
         <f t="shared" si="3"/>
         <v>-400</v>
       </c>
-      <c r="AF14" s="57">
+      <c r="AF14" s="54">
         <f t="shared" si="3"/>
         <v>-402</v>
       </c>
-      <c r="AG14" s="36">
+      <c r="AG14" s="35">
         <f t="shared" si="3"/>
         <v>-423</v>
       </c>
-      <c r="AH14" s="78">
+      <c r="AH14" s="70">
         <f t="shared" si="3"/>
         <v>-425</v>
       </c>
-      <c r="AI14" s="36">
+      <c r="AI14" s="35">
         <f t="shared" si="3"/>
         <v>-431</v>
       </c>
-      <c r="AJ14" s="37">
+      <c r="AJ14" s="36">
         <f t="shared" si="5"/>
         <v>-433</v>
       </c>
@@ -3025,102 +3184,90 @@
       <c r="AL14" s="30"/>
     </row>
     <row r="15" spans="1:40" ht="15.75" thickBot="1">
-      <c r="A15" s="19"/>
-      <c r="B15" s="123">
+      <c r="A15" s="131">
         <v>5</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="123">
+      <c r="B15" s="124"/>
+      <c r="C15" s="130">
         <v>5</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="123">
-        <v>5</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="122">
-        <v>5</v>
-      </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="123">
-        <v>5</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="123">
-        <v>5</v>
-      </c>
-      <c r="M15" s="1"/>
-      <c r="N15" s="123">
-        <v>5</v>
-      </c>
-      <c r="O15" s="1"/>
-      <c r="P15" s="122">
-        <v>5</v>
-      </c>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="125"/>
+      <c r="I15" s="123"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="124"/>
+      <c r="O15" s="124"/>
+      <c r="P15" s="125"/>
       <c r="Q15">
         <v>14</v>
       </c>
-      <c r="U15" s="86">
+      <c r="U15" s="129">
         <f t="shared" si="2"/>
         <v>-291</v>
       </c>
-      <c r="V15" s="101">
+      <c r="V15" s="93">
         <f t="shared" si="2"/>
         <v>-293</v>
       </c>
-      <c r="W15" s="88">
+      <c r="W15" s="128">
         <f t="shared" si="2"/>
         <v>-299</v>
       </c>
-      <c r="X15" s="87">
+      <c r="X15" s="79">
         <f t="shared" si="2"/>
         <v>-301</v>
       </c>
-      <c r="Y15" s="88">
+      <c r="Y15" s="80">
         <f t="shared" si="2"/>
         <v>-322</v>
       </c>
-      <c r="Z15" s="101">
+      <c r="Z15" s="93">
         <f t="shared" si="2"/>
         <v>-324</v>
       </c>
-      <c r="AA15" s="88">
+      <c r="AA15" s="80">
         <f t="shared" si="2"/>
         <v>-330</v>
       </c>
-      <c r="AB15" s="89">
+      <c r="AB15" s="81">
         <f t="shared" si="4"/>
         <v>-332</v>
       </c>
-      <c r="AC15" s="103">
+      <c r="AC15" s="95">
         <f t="shared" si="3"/>
         <v>-391</v>
       </c>
-      <c r="AD15" s="101">
+      <c r="AD15" s="93">
         <f t="shared" si="3"/>
         <v>-393</v>
       </c>
-      <c r="AE15" s="103">
+      <c r="AE15" s="95">
         <f t="shared" si="3"/>
         <v>-399</v>
       </c>
-      <c r="AF15" s="87">
+      <c r="AF15" s="79">
         <f t="shared" si="3"/>
         <v>-401</v>
       </c>
-      <c r="AG15" s="103">
+      <c r="AG15" s="95">
         <f t="shared" si="3"/>
         <v>-422</v>
       </c>
-      <c r="AH15" s="101">
+      <c r="AH15" s="93">
         <f t="shared" si="3"/>
         <v>-424</v>
       </c>
-      <c r="AI15" s="103">
+      <c r="AI15" s="95">
         <f t="shared" si="3"/>
         <v>-430</v>
       </c>
-      <c r="AJ15" s="104">
+      <c r="AJ15" s="96">
         <f t="shared" si="5"/>
         <v>-432</v>
       </c>
@@ -3148,67 +3295,67 @@
       <c r="Q16">
         <v>15</v>
       </c>
-      <c r="U16" s="45">
+      <c r="U16" s="44">
         <f t="shared" si="2"/>
         <v>-288</v>
       </c>
-      <c r="V16" s="78">
+      <c r="V16" s="70">
         <f t="shared" si="2"/>
         <v>-290</v>
       </c>
-      <c r="W16" s="51">
+      <c r="W16" s="50">
         <f t="shared" si="2"/>
         <v>-296</v>
       </c>
-      <c r="X16" s="57">
+      <c r="X16" s="54">
         <f t="shared" si="2"/>
         <v>-298</v>
       </c>
-      <c r="Y16" s="51">
+      <c r="Y16" s="50">
         <f t="shared" si="2"/>
         <v>-320</v>
       </c>
-      <c r="Z16" s="78">
+      <c r="Z16" s="70">
         <f t="shared" si="2"/>
         <v>-322</v>
       </c>
-      <c r="AA16" s="51">
+      <c r="AA16" s="50">
         <f t="shared" si="2"/>
         <v>-327</v>
       </c>
-      <c r="AB16" s="66">
+      <c r="AB16" s="61">
         <f t="shared" si="4"/>
         <v>-329</v>
       </c>
-      <c r="AC16" s="36">
+      <c r="AC16" s="35">
         <f t="shared" si="3"/>
         <v>-388</v>
       </c>
-      <c r="AD16" s="78">
+      <c r="AD16" s="70">
         <f t="shared" si="3"/>
         <v>-390</v>
       </c>
-      <c r="AE16" s="36">
+      <c r="AE16" s="35">
         <f t="shared" si="3"/>
         <v>-396</v>
       </c>
-      <c r="AF16" s="57">
+      <c r="AF16" s="54">
         <f t="shared" si="3"/>
         <v>-398</v>
       </c>
-      <c r="AG16" s="36">
+      <c r="AG16" s="35">
         <f t="shared" si="3"/>
         <v>-420</v>
       </c>
-      <c r="AH16" s="78">
+      <c r="AH16" s="70">
         <f t="shared" si="3"/>
         <v>-422</v>
       </c>
-      <c r="AI16" s="36">
+      <c r="AI16" s="35">
         <f t="shared" si="3"/>
         <v>-427</v>
       </c>
-      <c r="AJ16" s="37">
+      <c r="AJ16" s="36">
         <f t="shared" si="5"/>
         <v>-429</v>
       </c>
@@ -3219,7 +3366,7 @@
     <row r="17" spans="1:37" ht="15.75" thickBot="1">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="121">
+      <c r="C17" s="113">
         <v>4</v>
       </c>
       <c r="D17" s="10"/>
@@ -3227,7 +3374,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="10"/>
-      <c r="G17" s="121">
+      <c r="G17" s="113">
         <v>4</v>
       </c>
       <c r="H17" s="16"/>
@@ -3235,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="10"/>
-      <c r="K17" s="121">
+      <c r="K17" s="113">
         <v>4</v>
       </c>
       <c r="L17" s="10"/>
@@ -3243,7 +3390,7 @@
         <v>2</v>
       </c>
       <c r="N17" s="10"/>
-      <c r="O17" s="121">
+      <c r="O17" s="113">
         <v>4</v>
       </c>
       <c r="P17" s="11"/>
@@ -3254,59 +3401,59 @@
         <f t="shared" si="2"/>
         <v>-287</v>
       </c>
-      <c r="V17" s="79">
+      <c r="V17" s="71">
         <f t="shared" si="2"/>
         <v>-289</v>
       </c>
-      <c r="W17" s="50">
+      <c r="W17" s="117">
         <f t="shared" si="2"/>
         <v>-295</v>
       </c>
-      <c r="X17" s="55">
+      <c r="X17" s="52">
         <f t="shared" si="2"/>
         <v>-297</v>
       </c>
-      <c r="Y17" s="114">
+      <c r="Y17" s="106">
         <f t="shared" si="2"/>
         <v>-319</v>
       </c>
-      <c r="Z17" s="79">
+      <c r="Z17" s="71">
         <f t="shared" si="2"/>
         <v>-321</v>
       </c>
-      <c r="AA17" s="50">
+      <c r="AA17" s="117">
         <f t="shared" si="2"/>
         <v>-326</v>
       </c>
-      <c r="AB17" s="64">
+      <c r="AB17" s="59">
         <f t="shared" si="4"/>
         <v>-328</v>
       </c>
-      <c r="AC17" s="111">
+      <c r="AC17" s="103">
         <f t="shared" si="3"/>
         <v>-387</v>
       </c>
-      <c r="AD17" s="79">
+      <c r="AD17" s="71">
         <f t="shared" si="3"/>
         <v>-389</v>
       </c>
-      <c r="AE17" s="34">
+      <c r="AE17" s="122">
         <f t="shared" si="3"/>
         <v>-395</v>
       </c>
-      <c r="AF17" s="55">
+      <c r="AF17" s="52">
         <f t="shared" si="3"/>
         <v>-397</v>
       </c>
-      <c r="AG17" s="115">
+      <c r="AG17" s="107">
         <f t="shared" si="3"/>
         <v>-419</v>
       </c>
-      <c r="AH17" s="79">
+      <c r="AH17" s="71">
         <f t="shared" si="3"/>
         <v>-421</v>
       </c>
-      <c r="AI17" s="34">
+      <c r="AI17" s="122">
         <f t="shared" si="3"/>
         <v>-426</v>
       </c>
@@ -3346,6 +3493,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Matrix search (ex5.) fully working solution.
</commit_message>
<xml_diff>
--- a/20441/maman16/Drawing.xlsx
+++ b/20441/maman16/Drawing.xlsx
@@ -315,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="75">
+  <borders count="110">
     <border>
       <left/>
       <right/>
@@ -1304,6 +1304,371 @@
       </top>
       <bottom style="thick">
         <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1311,7 +1676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1617,6 +1982,42 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="96" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="98" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="100" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="101" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="102" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="103" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="104" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="105" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="106" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="109" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1912,10 +2313,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AN20"/>
+  <dimension ref="A1:AN36"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AJ36" sqref="AJ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
@@ -1923,9 +2324,13 @@
     <col min="1" max="7" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.5703125" style="21"/>
     <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="19" max="19" width="3.5703125" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" customWidth="1"/>
     <col min="21" max="28" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="5" style="31" bestFit="1" customWidth="1"/>
-    <col min="30" max="36" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="36" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1979,16 +2384,16 @@
         <v>1</v>
       </c>
       <c r="U1" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="V1" s="3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="W1" s="3">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="X1" s="3">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="Y1" s="3">
         <v>12</v>
@@ -2217,7 +2622,7 @@
       </c>
       <c r="W4" s="50">
         <f t="shared" si="0"/>
-        <v>-363</v>
+        <v>-362</v>
       </c>
       <c r="X4" s="54">
         <f t="shared" si="0"/>
@@ -2246,7 +2651,7 @@
         <v>-456</v>
       </c>
       <c r="AE4" s="73">
-        <v>-463</v>
+        <v>-462</v>
       </c>
       <c r="AF4" s="74">
         <v>-464</v>
@@ -2318,7 +2723,7 @@
       </c>
       <c r="X5" s="53">
         <f t="shared" si="0"/>
-        <v>-362</v>
+        <v>-363</v>
       </c>
       <c r="Y5" s="109">
         <f t="shared" si="0"/>
@@ -2346,7 +2751,7 @@
         <v>-461</v>
       </c>
       <c r="AF5" s="57">
-        <v>-462</v>
+        <v>-463</v>
       </c>
       <c r="AG5" s="108">
         <v>-484</v>
@@ -2928,7 +3333,7 @@
       </c>
       <c r="W12" s="50">
         <f t="shared" si="2"/>
-        <v>-313</v>
+        <v>-312</v>
       </c>
       <c r="X12" s="54">
         <f t="shared" si="2"/>
@@ -2960,7 +3365,7 @@
       </c>
       <c r="AE12" s="35">
         <f t="shared" si="3"/>
-        <v>-413</v>
+        <v>-412</v>
       </c>
       <c r="AF12" s="54">
         <f t="shared" si="3"/>
@@ -3038,7 +3443,7 @@
       </c>
       <c r="X13" s="53">
         <f t="shared" si="2"/>
-        <v>-312</v>
+        <v>-313</v>
       </c>
       <c r="Y13" s="109">
         <f t="shared" si="2"/>
@@ -3070,7 +3475,7 @@
       </c>
       <c r="AF13" s="53">
         <f t="shared" si="3"/>
-        <v>-412</v>
+        <v>-413</v>
       </c>
       <c r="AG13" s="111">
         <f t="shared" si="3"/>
@@ -3472,20 +3877,953 @@
       <c r="Y18" s="22"/>
       <c r="Z18" s="22"/>
     </row>
-    <row r="19" spans="1:37">
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22"/>
-      <c r="Z19" s="22"/>
+    <row r="19" spans="1:37" ht="15.75" thickBot="1">
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>2</v>
+      </c>
+      <c r="W19">
+        <v>3</v>
+      </c>
+      <c r="X19">
+        <v>4</v>
+      </c>
+      <c r="Y19">
+        <v>5</v>
+      </c>
+      <c r="Z19">
+        <v>6</v>
+      </c>
+      <c r="AA19">
+        <v>7</v>
+      </c>
+      <c r="AB19">
+        <v>8</v>
+      </c>
+      <c r="AC19">
+        <v>9</v>
+      </c>
+      <c r="AD19">
+        <v>10</v>
+      </c>
+      <c r="AE19">
+        <v>11</v>
+      </c>
+      <c r="AF19">
+        <v>12</v>
+      </c>
+      <c r="AG19">
+        <v>13</v>
+      </c>
+      <c r="AH19">
+        <v>14</v>
+      </c>
+      <c r="AI19">
+        <v>15</v>
+      </c>
+      <c r="AJ19">
+        <v>16</v>
+      </c>
     </row>
-    <row r="20" spans="1:37">
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="22"/>
+    <row r="20" spans="1:37" ht="15.75" thickTop="1">
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20" s="133">
+        <v>1</v>
+      </c>
+      <c r="V20" s="157">
+        <v>3</v>
+      </c>
+      <c r="W20" s="134">
+        <v>9</v>
+      </c>
+      <c r="X20" s="147">
+        <v>11</v>
+      </c>
+      <c r="Y20" s="134">
+        <v>33</v>
+      </c>
+      <c r="Z20" s="157">
+        <v>35</v>
+      </c>
+      <c r="AA20" s="134">
+        <v>41</v>
+      </c>
+      <c r="AB20" s="140">
+        <v>43</v>
+      </c>
+      <c r="AC20" s="134">
+        <v>129</v>
+      </c>
+      <c r="AD20" s="157">
+        <v>131</v>
+      </c>
+      <c r="AE20" s="134">
+        <v>137</v>
+      </c>
+      <c r="AF20" s="147">
+        <v>139</v>
+      </c>
+      <c r="AG20" s="134">
+        <v>161</v>
+      </c>
+      <c r="AH20" s="157">
+        <v>163</v>
+      </c>
+      <c r="AI20" s="134">
+        <v>169</v>
+      </c>
+      <c r="AJ20" s="135">
+        <v>171</v>
+      </c>
     </row>
+    <row r="21" spans="1:37" ht="15.75" thickBot="1">
+      <c r="T21">
+        <v>2</v>
+      </c>
+      <c r="U21" s="162">
+        <v>2</v>
+      </c>
+      <c r="V21" s="163">
+        <v>4</v>
+      </c>
+      <c r="W21" s="164">
+        <v>10</v>
+      </c>
+      <c r="X21" s="165">
+        <v>12</v>
+      </c>
+      <c r="Y21" s="164">
+        <v>34</v>
+      </c>
+      <c r="Z21" s="163">
+        <v>36</v>
+      </c>
+      <c r="AA21" s="164">
+        <v>42</v>
+      </c>
+      <c r="AB21" s="166">
+        <v>44</v>
+      </c>
+      <c r="AC21" s="164">
+        <v>130</v>
+      </c>
+      <c r="AD21" s="163">
+        <v>132</v>
+      </c>
+      <c r="AE21" s="164">
+        <v>138</v>
+      </c>
+      <c r="AF21" s="165">
+        <v>140</v>
+      </c>
+      <c r="AG21" s="164">
+        <v>162</v>
+      </c>
+      <c r="AH21" s="163">
+        <v>164</v>
+      </c>
+      <c r="AI21" s="164">
+        <v>170</v>
+      </c>
+      <c r="AJ21" s="167">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" ht="15.75" thickTop="1">
+      <c r="T22">
+        <v>3</v>
+      </c>
+      <c r="U22" s="136">
+        <v>5</v>
+      </c>
+      <c r="V22" s="158">
+        <v>7</v>
+      </c>
+      <c r="W22" s="168">
+        <v>13</v>
+      </c>
+      <c r="X22" s="148">
+        <v>15</v>
+      </c>
+      <c r="Y22" s="168">
+        <v>37</v>
+      </c>
+      <c r="Z22" s="158">
+        <v>39</v>
+      </c>
+      <c r="AA22" s="168">
+        <v>45</v>
+      </c>
+      <c r="AB22" s="141">
+        <v>47</v>
+      </c>
+      <c r="AC22" s="168">
+        <v>133</v>
+      </c>
+      <c r="AD22" s="158">
+        <v>135</v>
+      </c>
+      <c r="AE22" s="168">
+        <v>141</v>
+      </c>
+      <c r="AF22" s="148">
+        <v>143</v>
+      </c>
+      <c r="AG22" s="168">
+        <v>165</v>
+      </c>
+      <c r="AH22" s="158">
+        <v>167</v>
+      </c>
+      <c r="AI22" s="168">
+        <v>173</v>
+      </c>
+      <c r="AJ22" s="137">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" ht="15.75" thickBot="1">
+      <c r="T23">
+        <v>4</v>
+      </c>
+      <c r="U23" s="150">
+        <v>6</v>
+      </c>
+      <c r="V23" s="159">
+        <v>8</v>
+      </c>
+      <c r="W23" s="151">
+        <v>14</v>
+      </c>
+      <c r="X23" s="152">
+        <v>16</v>
+      </c>
+      <c r="Y23" s="151">
+        <v>38</v>
+      </c>
+      <c r="Z23" s="159">
+        <v>40</v>
+      </c>
+      <c r="AA23" s="151">
+        <v>46</v>
+      </c>
+      <c r="AB23" s="153">
+        <v>48</v>
+      </c>
+      <c r="AC23" s="151">
+        <v>134</v>
+      </c>
+      <c r="AD23" s="159">
+        <v>136</v>
+      </c>
+      <c r="AE23" s="151">
+        <v>142</v>
+      </c>
+      <c r="AF23" s="152">
+        <v>144</v>
+      </c>
+      <c r="AG23" s="151">
+        <v>166</v>
+      </c>
+      <c r="AH23" s="159">
+        <v>168</v>
+      </c>
+      <c r="AI23" s="151">
+        <v>174</v>
+      </c>
+      <c r="AJ23" s="154">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" ht="15.75" thickTop="1">
+      <c r="T24">
+        <v>5</v>
+      </c>
+      <c r="U24" s="136">
+        <v>17</v>
+      </c>
+      <c r="V24" s="158">
+        <v>19</v>
+      </c>
+      <c r="W24" s="168">
+        <v>25</v>
+      </c>
+      <c r="X24" s="148">
+        <v>27</v>
+      </c>
+      <c r="Y24" s="168">
+        <v>49</v>
+      </c>
+      <c r="Z24" s="158">
+        <v>51</v>
+      </c>
+      <c r="AA24" s="168">
+        <v>57</v>
+      </c>
+      <c r="AB24" s="141">
+        <v>59</v>
+      </c>
+      <c r="AC24" s="168">
+        <v>145</v>
+      </c>
+      <c r="AD24" s="158">
+        <v>147</v>
+      </c>
+      <c r="AE24" s="168">
+        <v>153</v>
+      </c>
+      <c r="AF24" s="148">
+        <v>155</v>
+      </c>
+      <c r="AG24" s="168">
+        <v>177</v>
+      </c>
+      <c r="AH24" s="158">
+        <v>179</v>
+      </c>
+      <c r="AI24" s="168">
+        <v>185</v>
+      </c>
+      <c r="AJ24" s="137">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" ht="15.75" thickBot="1">
+      <c r="L25" s="168">
+        <v>81</v>
+      </c>
+      <c r="M25" s="158">
+        <v>83</v>
+      </c>
+      <c r="N25" s="168">
+        <v>89</v>
+      </c>
+      <c r="O25" s="141">
+        <v>91</v>
+      </c>
+      <c r="T25">
+        <v>6</v>
+      </c>
+      <c r="U25" s="162">
+        <v>18</v>
+      </c>
+      <c r="V25" s="163">
+        <v>20</v>
+      </c>
+      <c r="W25" s="164">
+        <v>26</v>
+      </c>
+      <c r="X25" s="165">
+        <v>28</v>
+      </c>
+      <c r="Y25" s="164">
+        <v>50</v>
+      </c>
+      <c r="Z25" s="163">
+        <v>52</v>
+      </c>
+      <c r="AA25" s="164">
+        <v>58</v>
+      </c>
+      <c r="AB25" s="166">
+        <v>60</v>
+      </c>
+      <c r="AC25" s="164">
+        <v>146</v>
+      </c>
+      <c r="AD25" s="163">
+        <v>148</v>
+      </c>
+      <c r="AE25" s="164">
+        <v>154</v>
+      </c>
+      <c r="AF25" s="165">
+        <v>156</v>
+      </c>
+      <c r="AG25" s="164">
+        <v>178</v>
+      </c>
+      <c r="AH25" s="163">
+        <v>180</v>
+      </c>
+      <c r="AI25" s="164">
+        <v>186</v>
+      </c>
+      <c r="AJ25" s="167">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" ht="16.5" thickTop="1" thickBot="1">
+      <c r="L26" s="164">
+        <v>82</v>
+      </c>
+      <c r="M26" s="163">
+        <v>84</v>
+      </c>
+      <c r="N26" s="164">
+        <v>90</v>
+      </c>
+      <c r="O26" s="166">
+        <v>92</v>
+      </c>
+      <c r="T26">
+        <v>7</v>
+      </c>
+      <c r="U26" s="136">
+        <v>21</v>
+      </c>
+      <c r="V26" s="158">
+        <v>23</v>
+      </c>
+      <c r="W26" s="168">
+        <v>29</v>
+      </c>
+      <c r="X26" s="148">
+        <v>31</v>
+      </c>
+      <c r="Y26" s="168">
+        <v>53</v>
+      </c>
+      <c r="Z26" s="158">
+        <v>55</v>
+      </c>
+      <c r="AA26" s="168">
+        <v>61</v>
+      </c>
+      <c r="AB26" s="141">
+        <v>63</v>
+      </c>
+      <c r="AC26" s="168">
+        <v>149</v>
+      </c>
+      <c r="AD26" s="158">
+        <v>151</v>
+      </c>
+      <c r="AE26" s="168">
+        <v>157</v>
+      </c>
+      <c r="AF26" s="148">
+        <v>159</v>
+      </c>
+      <c r="AG26" s="168">
+        <v>181</v>
+      </c>
+      <c r="AH26" s="158">
+        <v>183</v>
+      </c>
+      <c r="AI26" s="168">
+        <v>189</v>
+      </c>
+      <c r="AJ26" s="137">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" ht="16.5" thickTop="1" thickBot="1">
+      <c r="L27" s="168">
+        <v>85</v>
+      </c>
+      <c r="M27" s="158">
+        <v>86</v>
+      </c>
+      <c r="N27" s="168">
+        <v>93</v>
+      </c>
+      <c r="O27" s="141">
+        <v>95</v>
+      </c>
+      <c r="T27">
+        <v>8</v>
+      </c>
+      <c r="U27" s="143">
+        <v>22</v>
+      </c>
+      <c r="V27" s="160">
+        <v>24</v>
+      </c>
+      <c r="W27" s="144">
+        <v>30</v>
+      </c>
+      <c r="X27" s="149">
+        <v>32</v>
+      </c>
+      <c r="Y27" s="144">
+        <v>54</v>
+      </c>
+      <c r="Z27" s="160">
+        <v>56</v>
+      </c>
+      <c r="AA27" s="144">
+        <v>62</v>
+      </c>
+      <c r="AB27" s="145">
+        <v>64</v>
+      </c>
+      <c r="AC27" s="144">
+        <v>150</v>
+      </c>
+      <c r="AD27" s="160">
+        <v>152</v>
+      </c>
+      <c r="AE27" s="144">
+        <v>158</v>
+      </c>
+      <c r="AF27" s="149">
+        <v>160</v>
+      </c>
+      <c r="AG27" s="144">
+        <v>182</v>
+      </c>
+      <c r="AH27" s="160">
+        <v>184</v>
+      </c>
+      <c r="AI27" s="144">
+        <v>190</v>
+      </c>
+      <c r="AJ27" s="146">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" ht="16.5" thickTop="1" thickBot="1">
+      <c r="L28" s="151">
+        <v>86</v>
+      </c>
+      <c r="M28" s="159">
+        <v>88</v>
+      </c>
+      <c r="N28" s="151">
+        <v>94</v>
+      </c>
+      <c r="O28" s="153">
+        <v>96</v>
+      </c>
+      <c r="T28">
+        <v>9</v>
+      </c>
+      <c r="U28" s="136">
+        <v>65</v>
+      </c>
+      <c r="V28" s="158">
+        <v>67</v>
+      </c>
+      <c r="W28" s="168">
+        <v>73</v>
+      </c>
+      <c r="X28" s="155">
+        <v>75</v>
+      </c>
+      <c r="Y28" s="168">
+        <v>97</v>
+      </c>
+      <c r="Z28" s="158">
+        <v>99</v>
+      </c>
+      <c r="AA28" s="168">
+        <v>105</v>
+      </c>
+      <c r="AB28" s="141">
+        <v>107</v>
+      </c>
+      <c r="AC28" s="168">
+        <v>193</v>
+      </c>
+      <c r="AD28" s="158">
+        <v>195</v>
+      </c>
+      <c r="AE28" s="168">
+        <v>201</v>
+      </c>
+      <c r="AF28" s="148">
+        <v>203</v>
+      </c>
+      <c r="AG28" s="168">
+        <v>225</v>
+      </c>
+      <c r="AH28" s="158">
+        <v>227</v>
+      </c>
+      <c r="AI28" s="168">
+        <v>233</v>
+      </c>
+      <c r="AJ28" s="137">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" ht="16.5" thickTop="1" thickBot="1">
+      <c r="T29">
+        <v>10</v>
+      </c>
+      <c r="U29" s="162">
+        <v>66</v>
+      </c>
+      <c r="V29" s="163">
+        <v>68</v>
+      </c>
+      <c r="W29" s="164">
+        <v>74</v>
+      </c>
+      <c r="X29" s="165">
+        <v>76</v>
+      </c>
+      <c r="Y29" s="164">
+        <v>98</v>
+      </c>
+      <c r="Z29" s="163">
+        <v>100</v>
+      </c>
+      <c r="AA29" s="164">
+        <v>106</v>
+      </c>
+      <c r="AB29" s="166">
+        <v>108</v>
+      </c>
+      <c r="AC29" s="164">
+        <v>194</v>
+      </c>
+      <c r="AD29" s="163">
+        <v>196</v>
+      </c>
+      <c r="AE29" s="164">
+        <v>202</v>
+      </c>
+      <c r="AF29" s="165">
+        <v>204</v>
+      </c>
+      <c r="AG29" s="164">
+        <v>226</v>
+      </c>
+      <c r="AH29" s="163">
+        <v>228</v>
+      </c>
+      <c r="AI29" s="164">
+        <v>234</v>
+      </c>
+      <c r="AJ29" s="167">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" ht="15.75" thickTop="1">
+      <c r="T30">
+        <v>11</v>
+      </c>
+      <c r="U30" s="136">
+        <v>69</v>
+      </c>
+      <c r="V30" s="158">
+        <v>71</v>
+      </c>
+      <c r="W30" s="168">
+        <v>77</v>
+      </c>
+      <c r="X30" s="148">
+        <v>79</v>
+      </c>
+      <c r="Y30" s="168">
+        <v>101</v>
+      </c>
+      <c r="Z30" s="158">
+        <v>103</v>
+      </c>
+      <c r="AA30" s="168">
+        <v>109</v>
+      </c>
+      <c r="AB30" s="141">
+        <v>111</v>
+      </c>
+      <c r="AC30" s="168">
+        <v>197</v>
+      </c>
+      <c r="AD30" s="158">
+        <v>199</v>
+      </c>
+      <c r="AE30" s="168">
+        <v>205</v>
+      </c>
+      <c r="AF30" s="148">
+        <v>207</v>
+      </c>
+      <c r="AG30" s="168">
+        <v>229</v>
+      </c>
+      <c r="AH30" s="158">
+        <v>231</v>
+      </c>
+      <c r="AI30" s="168">
+        <v>237</v>
+      </c>
+      <c r="AJ30" s="137">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" ht="15.75" thickBot="1">
+      <c r="T31">
+        <v>12</v>
+      </c>
+      <c r="U31" s="150">
+        <v>70</v>
+      </c>
+      <c r="V31" s="159">
+        <v>72</v>
+      </c>
+      <c r="W31" s="151">
+        <v>78</v>
+      </c>
+      <c r="X31" s="152">
+        <v>80</v>
+      </c>
+      <c r="Y31" s="151">
+        <v>102</v>
+      </c>
+      <c r="Z31" s="159">
+        <v>104</v>
+      </c>
+      <c r="AA31" s="151">
+        <v>110</v>
+      </c>
+      <c r="AB31" s="153">
+        <v>112</v>
+      </c>
+      <c r="AC31" s="151">
+        <v>198</v>
+      </c>
+      <c r="AD31" s="159">
+        <v>200</v>
+      </c>
+      <c r="AE31" s="151">
+        <v>206</v>
+      </c>
+      <c r="AF31" s="152">
+        <v>208</v>
+      </c>
+      <c r="AG31" s="151">
+        <v>230</v>
+      </c>
+      <c r="AH31" s="159">
+        <v>232</v>
+      </c>
+      <c r="AI31" s="151">
+        <v>238</v>
+      </c>
+      <c r="AJ31" s="154">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" ht="15.75" thickTop="1">
+      <c r="T32">
+        <v>13</v>
+      </c>
+      <c r="U32" s="168">
+        <v>81</v>
+      </c>
+      <c r="V32" s="158">
+        <v>83</v>
+      </c>
+      <c r="W32" s="168">
+        <v>89</v>
+      </c>
+      <c r="X32" s="141">
+        <v>91</v>
+      </c>
+      <c r="Y32" s="168">
+        <v>113</v>
+      </c>
+      <c r="Z32" s="158">
+        <v>115</v>
+      </c>
+      <c r="AA32" s="168">
+        <v>121</v>
+      </c>
+      <c r="AB32" s="141">
+        <v>123</v>
+      </c>
+      <c r="AC32" s="168">
+        <v>209</v>
+      </c>
+      <c r="AD32" s="158">
+        <v>211</v>
+      </c>
+      <c r="AE32" s="168">
+        <v>217</v>
+      </c>
+      <c r="AF32" s="148">
+        <v>219</v>
+      </c>
+      <c r="AG32" s="168">
+        <v>241</v>
+      </c>
+      <c r="AH32" s="158">
+        <v>243</v>
+      </c>
+      <c r="AI32" s="168">
+        <v>249</v>
+      </c>
+      <c r="AJ32" s="137">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="20:36" ht="15.75" thickBot="1">
+      <c r="T33">
+        <v>14</v>
+      </c>
+      <c r="U33" s="164">
+        <v>82</v>
+      </c>
+      <c r="V33" s="163">
+        <v>84</v>
+      </c>
+      <c r="W33" s="164">
+        <v>90</v>
+      </c>
+      <c r="X33" s="166">
+        <v>92</v>
+      </c>
+      <c r="Y33" s="164">
+        <v>114</v>
+      </c>
+      <c r="Z33" s="163">
+        <v>116</v>
+      </c>
+      <c r="AA33" s="164">
+        <v>122</v>
+      </c>
+      <c r="AB33" s="166">
+        <v>124</v>
+      </c>
+      <c r="AC33" s="164">
+        <v>210</v>
+      </c>
+      <c r="AD33" s="163">
+        <v>212</v>
+      </c>
+      <c r="AE33" s="164">
+        <v>218</v>
+      </c>
+      <c r="AF33" s="165">
+        <v>220</v>
+      </c>
+      <c r="AG33" s="164">
+        <v>242</v>
+      </c>
+      <c r="AH33" s="163">
+        <v>244</v>
+      </c>
+      <c r="AI33" s="164">
+        <v>250</v>
+      </c>
+      <c r="AJ33" s="167">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="20:36" ht="15.75" thickTop="1">
+      <c r="T34">
+        <v>15</v>
+      </c>
+      <c r="U34" s="168">
+        <v>85</v>
+      </c>
+      <c r="V34" s="158">
+        <v>86</v>
+      </c>
+      <c r="W34" s="168">
+        <v>93</v>
+      </c>
+      <c r="X34" s="141">
+        <v>95</v>
+      </c>
+      <c r="Y34" s="168">
+        <v>117</v>
+      </c>
+      <c r="Z34" s="158">
+        <v>119</v>
+      </c>
+      <c r="AA34" s="168">
+        <v>125</v>
+      </c>
+      <c r="AB34" s="141">
+        <v>127</v>
+      </c>
+      <c r="AC34" s="168">
+        <v>213</v>
+      </c>
+      <c r="AD34" s="158">
+        <v>215</v>
+      </c>
+      <c r="AE34" s="168">
+        <v>221</v>
+      </c>
+      <c r="AF34" s="148">
+        <v>223</v>
+      </c>
+      <c r="AG34" s="168">
+        <v>245</v>
+      </c>
+      <c r="AH34" s="158">
+        <v>247</v>
+      </c>
+      <c r="AI34" s="168">
+        <v>253</v>
+      </c>
+      <c r="AJ34" s="137">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="20:36" ht="15.75" thickBot="1">
+      <c r="T35">
+        <v>16</v>
+      </c>
+      <c r="U35" s="151">
+        <v>86</v>
+      </c>
+      <c r="V35" s="159">
+        <v>88</v>
+      </c>
+      <c r="W35" s="151">
+        <v>94</v>
+      </c>
+      <c r="X35" s="153">
+        <v>96</v>
+      </c>
+      <c r="Y35" s="138">
+        <v>118</v>
+      </c>
+      <c r="Z35" s="161">
+        <v>120</v>
+      </c>
+      <c r="AA35" s="138">
+        <v>126</v>
+      </c>
+      <c r="AB35" s="142">
+        <v>128</v>
+      </c>
+      <c r="AC35" s="138">
+        <v>214</v>
+      </c>
+      <c r="AD35" s="161">
+        <v>216</v>
+      </c>
+      <c r="AE35" s="138">
+        <v>222</v>
+      </c>
+      <c r="AF35" s="156">
+        <v>224</v>
+      </c>
+      <c r="AG35" s="138">
+        <v>246</v>
+      </c>
+      <c r="AH35" s="161">
+        <v>248</v>
+      </c>
+      <c r="AI35" s="138">
+        <v>254</v>
+      </c>
+      <c r="AJ35" s="139">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="20:36" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="R8:R14"/>

</xml_diff>